<commit_message>
Round1: Filter compounds with Chemspider logPs.
</commit_message>
<xml_diff>
--- a/compound_selection/zinc15_eMolecules_intersection_set/20170807_zinc15_eMolecules_subset_depiction/df_frag_final_oe.xlsx
+++ b/compound_selection/zinc15_eMolecules_intersection_set/20170807_zinc15_eMolecules_subset_depiction/df_frag_final_oe.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="392" uniqueCount="237">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="392" uniqueCount="233">
   <si>
     <t>df_frag_final_oe.csv</t>
   </si>
@@ -67,630 +67,645 @@
     <t>eMolecules ID</t>
   </si>
   <si>
-    <t>COc1ccc2c(c1)oc(=O)cc2CC(=O)O</t>
-  </si>
-  <si>
-    <t>[3.621]</t>
-  </si>
-  <si>
-    <t>0.6690000891685486</t>
-  </si>
-  <si>
-    <t>234.205</t>
-  </si>
-  <si>
-    <t>3439.8</t>
+    <t>Oc1cc2c3CCCNC(=O)c3oc2cc1</t>
+  </si>
+  <si>
+    <t>[9.119]</t>
+  </si>
+  <si>
+    <t>0.7199999690055847</t>
+  </si>
+  <si>
+    <t>217.221</t>
+  </si>
+  <si>
+    <t>184.0</t>
+  </si>
+  <si>
+    <t>533.0</t>
+  </si>
+  <si>
+    <t>fragment-like</t>
+  </si>
+  <si>
+    <t>0</t>
+  </si>
+  <si>
+    <t>27</t>
+  </si>
+  <si>
+    <t>picked</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>True</t>
+  </si>
+  <si>
+    <t>c1cc2c(cc1O)c3c(o2)C(=O)NCCC3</t>
+  </si>
+  <si>
+    <t>6679830</t>
+  </si>
+  <si>
+    <t>Nc1ncnc2c1cnn2c1ccccc1</t>
+  </si>
+  <si>
+    <t>[3.869]</t>
+  </si>
+  <si>
+    <t>1.4990001916885376</t>
+  </si>
+  <si>
+    <t>211.223</t>
+  </si>
+  <si>
+    <t>3430.0</t>
+  </si>
+  <si>
+    <t>414.0</t>
+  </si>
+  <si>
+    <t>31</t>
+  </si>
+  <si>
+    <t>8</t>
+  </si>
+  <si>
+    <t>c1ccc(cc1)n2c3c(cn2)c(ncn3)N</t>
+  </si>
+  <si>
+    <t>719540</t>
+  </si>
+  <si>
+    <t>O=C(c1ccccc1)Nc1ccncc1</t>
+  </si>
+  <si>
+    <t>[4.714]</t>
+  </si>
+  <si>
+    <t>1.694999933242798</t>
+  </si>
+  <si>
+    <t>198.221</t>
+  </si>
+  <si>
+    <t>116.0</t>
+  </si>
+  <si>
+    <t>168.0</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>20</t>
+  </si>
+  <si>
+    <t>9</t>
+  </si>
+  <si>
+    <t>c1ccc(cc1)C(=O)Nc2ccncc2</t>
+  </si>
+  <si>
+    <t>45490344</t>
+  </si>
+  <si>
+    <t>CSc1ccc(cc1)/C=C\1/NC(=O)NC1=O</t>
+  </si>
+  <si>
+    <t>[8.74]</t>
+  </si>
+  <si>
+    <t>1.8569998741149905</t>
+  </si>
+  <si>
+    <t>234.274</t>
+  </si>
+  <si>
+    <t>135.0</t>
+  </si>
+  <si>
+    <t>355.0</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>12</t>
+  </si>
+  <si>
+    <t>CSc1ccc(cc1)/C=C/2\C(=O)NC(=O)N2</t>
+  </si>
+  <si>
+    <t>27013168</t>
+  </si>
+  <si>
+    <t>Oc1ccc(cc1)n1cnc2c1cccc2</t>
+  </si>
+  <si>
+    <t>[5.82, 8.709]</t>
+  </si>
+  <si>
+    <t>2.2190003395080566</t>
+  </si>
+  <si>
+    <t>210.231</t>
+  </si>
+  <si>
+    <t>21650.2</t>
+  </si>
+  <si>
+    <t>148.0</t>
+  </si>
+  <si>
+    <t>40</t>
+  </si>
+  <si>
+    <t>11</t>
+  </si>
+  <si>
+    <t>c1ccc2c(c1)ncn2c3ccc(cc3)O</t>
+  </si>
+  <si>
+    <t>37095168</t>
+  </si>
+  <si>
+    <t>NC(=O)c1ccc2c(c1)nc([nH]2)c1ccccc1</t>
+  </si>
+  <si>
+    <t>[6.342]</t>
+  </si>
+  <si>
+    <t>2.1920003890991206</t>
+  </si>
+  <si>
+    <t>237.257</t>
+  </si>
+  <si>
+    <t>2000.0</t>
+  </si>
+  <si>
+    <t>42</t>
+  </si>
+  <si>
+    <t>c1ccc(cc1)c2[nH]c3ccc(cc3n2)C(=O)N</t>
+  </si>
+  <si>
+    <t>37053191</t>
+  </si>
+  <si>
+    <t>Nc1ccc2c(c1)ncn2c1ccccc1</t>
+  </si>
+  <si>
+    <t>[6.348]</t>
+  </si>
+  <si>
+    <t>2.3329999446868896</t>
+  </si>
+  <si>
+    <t>209.247</t>
+  </si>
+  <si>
+    <t>50213.0</t>
+  </si>
+  <si>
+    <t>c1ccc(cc1)n2cnc3c2ccc(c3)N</t>
+  </si>
+  <si>
+    <t>31653344</t>
+  </si>
+  <si>
+    <t>Nc1nonc1c1nc2c(n1CC1CC1)cccc2</t>
+  </si>
+  <si>
+    <t>[4.082]</t>
+  </si>
+  <si>
+    <t>2.43999981880188</t>
+  </si>
+  <si>
+    <t>255.275</t>
+  </si>
+  <si>
+    <t>300.0</t>
+  </si>
+  <si>
+    <t>28</t>
+  </si>
+  <si>
+    <t>c1ccc2c(c1)nc(n2CC3CC3)c4c(non4)N</t>
+  </si>
+  <si>
+    <t>8332960</t>
+  </si>
+  <si>
+    <t>O=C(c1n[nH]c2c1cccc2)Nc1ccccc1</t>
+  </si>
+  <si>
+    <t>[8.398]</t>
+  </si>
+  <si>
+    <t>2.6429998874664307</t>
+  </si>
+  <si>
+    <t>762.8</t>
   </si>
   <si>
     <t>223.0</t>
   </si>
   <si>
-    <t>fragment-like</t>
-  </si>
-  <si>
-    <t>3</t>
-  </si>
-  <si>
-    <t>29</t>
-  </si>
-  <si>
-    <t>picked</t>
-  </si>
-  <si>
-    <t>1</t>
-  </si>
-  <si>
-    <t>True</t>
-  </si>
-  <si>
-    <t>COc1ccc2c(cc(=O)oc2c1)CC(=O)O</t>
-  </si>
-  <si>
-    <t>490595</t>
-  </si>
-  <si>
-    <t>Oc1ccc(cc1)c1coc2c(c1=O)c(O)cc(c2)O</t>
-  </si>
-  <si>
-    <t>[8.584, 9.84, 10.869]</t>
-  </si>
-  <si>
-    <t>0.8870003223419191</t>
-  </si>
-  <si>
-    <t>270.237</t>
-  </si>
-  <si>
-    <t>1015.0</t>
-  </si>
-  <si>
-    <t>168.0</t>
-  </si>
-  <si>
-    <t>56</t>
-  </si>
-  <si>
-    <t>4</t>
-  </si>
-  <si>
-    <t>c1cc(ccc1c2coc3cc(cc(c3c2=O)O)O)O</t>
-  </si>
-  <si>
-    <t>532754</t>
-  </si>
-  <si>
-    <t>COC(=O)c1ccc(cc1)Nc1ncnc2c1nc[nH]2</t>
-  </si>
-  <si>
-    <t>[3.923, 9.999]</t>
-  </si>
-  <si>
-    <t>0.8499998450279236</t>
-  </si>
-  <si>
-    <t>269.259</t>
-  </si>
-  <si>
-    <t>108.0</t>
+    <t>36</t>
+  </si>
+  <si>
+    <t>13</t>
+  </si>
+  <si>
+    <t>c1ccc(cc1)NC(=O)c2c3ccccc3[nH]n2</t>
+  </si>
+  <si>
+    <t>13419113</t>
+  </si>
+  <si>
+    <t>Nc1ccc(cc1)c1nn2c(s1)nnc2C</t>
+  </si>
+  <si>
+    <t>[3.49, 5.213]</t>
+  </si>
+  <si>
+    <t>2.6009995937347408</t>
+  </si>
+  <si>
+    <t>231.277</t>
+  </si>
+  <si>
+    <t>13483.0</t>
   </si>
   <si>
     <t>275.0</t>
   </si>
   <si>
-    <t>20</t>
-  </si>
-  <si>
-    <t>2</t>
-  </si>
-  <si>
-    <t>COC(=O)c1ccc(cc1)Nc2c3c([nH]cn3)ncn2</t>
-  </si>
-  <si>
-    <t>4934119</t>
-  </si>
-  <si>
-    <t>Nc1ncnc2c1c1CCCc1s2</t>
-  </si>
-  <si>
-    <t>[4.048]</t>
-  </si>
-  <si>
-    <t>1.0429999828338623</t>
-  </si>
-  <si>
-    <t>191.253</t>
-  </si>
-  <si>
-    <t>1026.0</t>
-  </si>
-  <si>
-    <t>0</t>
-  </si>
-  <si>
-    <t>10</t>
+    <t>19</t>
+  </si>
+  <si>
+    <t>Cc1nnc2n1nc(s2)c3ccc(cc3)N</t>
+  </si>
+  <si>
+    <t>1503405</t>
+  </si>
+  <si>
+    <t>O=C(Nc1nc2c(s1)cccc2)CNC(=O)c1ccccc1</t>
+  </si>
+  <si>
+    <t>[8.672]</t>
+  </si>
+  <si>
+    <t>2.7179999351501465</t>
+  </si>
+  <si>
+    <t>311.358</t>
+  </si>
+  <si>
+    <t>149.1</t>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
+    <t>14</t>
+  </si>
+  <si>
+    <t>c1ccc(cc1)C(=O)NCC(=O)Nc2nc3ccccc3s2</t>
+  </si>
+  <si>
+    <t>23354217</t>
+  </si>
+  <si>
+    <t>O=C(c1c(F)cccc1Cl)Nc1ccncc1</t>
+  </si>
+  <si>
+    <t>[4.714, 10.192]</t>
+  </si>
+  <si>
+    <t>2.7859997749328613</t>
+  </si>
+  <si>
+    <t>250.656</t>
+  </si>
+  <si>
+    <t>115.0</t>
+  </si>
+  <si>
+    <t>c1cc(c(c(c1)Cl)C(=O)Nc2ccncc2)F</t>
+  </si>
+  <si>
+    <t>17004732</t>
+  </si>
+  <si>
+    <t>Brc1cncc(c1)C(=O)Nc1cccc2c1nccc2</t>
+  </si>
+  <si>
+    <t>[4.001, 10.328]</t>
+  </si>
+  <si>
+    <t>2.922999620437622</t>
+  </si>
+  <si>
+    <t>328.163</t>
+  </si>
+  <si>
+    <t>406.0</t>
+  </si>
+  <si>
+    <t>37</t>
+  </si>
+  <si>
+    <t>15</t>
+  </si>
+  <si>
+    <t>c1cc2cccnc2c(c1)NC(=O)c3cc(cnc3)Br</t>
+  </si>
+  <si>
+    <t>18893169</t>
+  </si>
+  <si>
+    <t>O=C(c1cccc(c1Cl)Cl)Nc1ccncc1</t>
+  </si>
+  <si>
+    <t>[4.714, 10.167]</t>
+  </si>
+  <si>
+    <t>2.9270002841949463</t>
+  </si>
+  <si>
+    <t>267.111</t>
+  </si>
+  <si>
+    <t>104.0</t>
+  </si>
+  <si>
+    <t>c1cc(c(c(c1)Cl)Cl)C(=O)Nc2ccncc2</t>
+  </si>
+  <si>
+    <t>2266357</t>
+  </si>
+  <si>
+    <t>COc1cccc(c1)Nc1ncnc2c1cccc2.Cl</t>
+  </si>
+  <si>
+    <t>[4.05]</t>
+  </si>
+  <si>
+    <t>3.138999938964844</t>
+  </si>
+  <si>
+    <t>287.744</t>
+  </si>
+  <si>
+    <t>119.7</t>
+  </si>
+  <si>
+    <t>16</t>
+  </si>
+  <si>
+    <t>COc1cccc(c1)Nc2c3ccccc3ncn2.Cl</t>
+  </si>
+  <si>
+    <t>1865544</t>
+  </si>
+  <si>
+    <t>c1ccc(cc1)n1cnc2c1cccc2</t>
+  </si>
+  <si>
+    <t>[5.74]</t>
+  </si>
+  <si>
+    <t>3.1050000190734863</t>
+  </si>
+  <si>
+    <t>194.232</t>
+  </si>
+  <si>
+    <t>188.0</t>
+  </si>
+  <si>
+    <t>c1ccc(cc1)n2cnc3c2cccc3</t>
+  </si>
+  <si>
+    <t>1202048</t>
+  </si>
+  <si>
+    <t>c1ccc(cc1)CSc1nnc(o1)c1ccncc1</t>
+  </si>
+  <si>
+    <t>[4.902]</t>
+  </si>
+  <si>
+    <t>3.3059999942779537</t>
+  </si>
+  <si>
+    <t>269.322</t>
+  </si>
+  <si>
+    <t>170.0</t>
+  </si>
+  <si>
+    <t>30</t>
+  </si>
+  <si>
+    <t>17</t>
+  </si>
+  <si>
+    <t>c1ccc(cc1)CSc2nnc(o2)c3ccncc3</t>
+  </si>
+  <si>
+    <t>1444229</t>
+  </si>
+  <si>
+    <t>O=C(c1ccc(cc1)Oc1ccccc1)NCc1ccncc1</t>
+  </si>
+  <si>
+    <t>[5.124]</t>
+  </si>
+  <si>
+    <t>3.2410001754760738</t>
+  </si>
+  <si>
+    <t>304.343</t>
+  </si>
+  <si>
+    <t>211.0</t>
+  </si>
+  <si>
+    <t>32</t>
+  </si>
+  <si>
+    <t>c1ccc(cc1)Oc2ccc(cc2)C(=O)NCc3ccncc3</t>
+  </si>
+  <si>
+    <t>3374919</t>
+  </si>
+  <si>
+    <t>O=C(c1cccs1)Nc1nnc(s1)Cc1ccccc1</t>
+  </si>
+  <si>
+    <t>[7.12]</t>
+  </si>
+  <si>
+    <t>3.6050002574920654</t>
+  </si>
+  <si>
+    <t>301.387</t>
+  </si>
+  <si>
+    <t>379.0</t>
   </si>
   <si>
     <t>5</t>
   </si>
   <si>
-    <t>c1nc(c2c3c(sc2n1)CCC3)N</t>
-  </si>
-  <si>
-    <t>2867544</t>
-  </si>
-  <si>
-    <t>Nc1ccc(c(c1)Nc1nccc(n1)c1cccnc1)C</t>
-  </si>
-  <si>
-    <t>[3.887, 4.98]</t>
-  </si>
-  <si>
-    <t>1.2969999313354492</t>
-  </si>
-  <si>
-    <t>277.324</t>
-  </si>
-  <si>
-    <t>101.1</t>
+    <t>18</t>
+  </si>
+  <si>
+    <t>c1ccc(cc1)Cc2nnc(s2)NC(=O)c3cccs3</t>
+  </si>
+  <si>
+    <t>1228629</t>
+  </si>
+  <si>
+    <t>Clc1ccc(cc1)CNc1ncnc2c1cccc2</t>
+  </si>
+  <si>
+    <t>[5.564]</t>
+  </si>
+  <si>
+    <t>3.523000240325928</t>
+  </si>
+  <si>
+    <t>269.72900000000004</t>
+  </si>
+  <si>
+    <t>415.5</t>
+  </si>
+  <si>
+    <t>c1ccc2c(c1)c(ncn2)NCc3ccc(cc3)Cl</t>
+  </si>
+  <si>
+    <t>30719859</t>
+  </si>
+  <si>
+    <t>Clc1ccc(o1)C(=O)Nc1ccccc1N1CCCCC1</t>
+  </si>
+  <si>
+    <t>[5.346]</t>
+  </si>
+  <si>
+    <t>3.794999837875366</t>
+  </si>
+  <si>
+    <t>304.771</t>
+  </si>
+  <si>
+    <t>424.3</t>
+  </si>
+  <si>
+    <t>c1ccc(c(c1)NC(=O)c2ccc(o2)Cl)N3CCCCC3</t>
+  </si>
+  <si>
+    <t>18908671</t>
+  </si>
+  <si>
+    <t>Cc1ccc(cc1)S(=O)(=O)Nc1cccc(c1)C(F)(F)F</t>
+  </si>
+  <si>
+    <t>[7.903]</t>
+  </si>
+  <si>
+    <t>3.747999668121338</t>
+  </si>
+  <si>
+    <t>315.311</t>
+  </si>
+  <si>
+    <t>527.0</t>
+  </si>
+  <si>
+    <t>24</t>
+  </si>
+  <si>
+    <t>Cc1ccc(cc1)S(=O)(=O)Nc2cccc(c2)C(F)(F)F</t>
+  </si>
+  <si>
+    <t>1377874</t>
+  </si>
+  <si>
+    <t>O=C1S/C(=C/c2ccc(o2)c2ccc(c(c2)Cl)F)/C(=O)N1</t>
+  </si>
+  <si>
+    <t>[8.052]</t>
+  </si>
+  <si>
+    <t>3.9079997539520255</t>
+  </si>
+  <si>
+    <t>323.7270000000001</t>
+  </si>
+  <si>
+    <t>125.0</t>
+  </si>
+  <si>
+    <t>c1cc(c(cc1c2ccc(o2)/C=C/3\C(=O)NC(=O)S3)Cl)F</t>
+  </si>
+  <si>
+    <t>25775231</t>
+  </si>
+  <si>
+    <t>FC(c1ccc(cc1)c1nnc2n1nc(cc2)NC1CC1)(F)F</t>
+  </si>
+  <si>
+    <t>[4.394]</t>
+  </si>
+  <si>
+    <t>4.128999710083009</t>
+  </si>
+  <si>
+    <t>319.284</t>
+  </si>
+  <si>
+    <t>3175.0</t>
+  </si>
+  <si>
+    <t>21</t>
+  </si>
+  <si>
+    <t>c1cc(ccc1c2nnc3n2nc(cc3)NC4CC4)C(F)(F)F</t>
+  </si>
+  <si>
+    <t>5784088</t>
+  </si>
+  <si>
+    <t>O=C1Nc2c(/C/1=C/c1ccc(cc1)C(C)C)cccc2</t>
+  </si>
+  <si>
+    <t>[3.158]</t>
+  </si>
+  <si>
+    <t>4.2330002784728995</t>
+  </si>
+  <si>
+    <t>263.334</t>
+  </si>
+  <si>
+    <t>283.7</t>
   </si>
   <si>
     <t>400.0</t>
   </si>
   <si>
-    <t>36</t>
-  </si>
-  <si>
-    <t>7</t>
-  </si>
-  <si>
-    <t>Cc1ccc(cc1Nc2nccc(n2)c3cccnc3)N</t>
-  </si>
-  <si>
-    <t>2727697</t>
-  </si>
-  <si>
-    <t>Nc1ncnc2c1cnn2c1ccccc1</t>
-  </si>
-  <si>
-    <t>[3.869]</t>
-  </si>
-  <si>
-    <t>1.4990001916885376</t>
-  </si>
-  <si>
-    <t>211.223</t>
-  </si>
-  <si>
-    <t>3430.0</t>
-  </si>
-  <si>
-    <t>414.0</t>
-  </si>
-  <si>
-    <t>31</t>
-  </si>
-  <si>
-    <t>8</t>
-  </si>
-  <si>
-    <t>c1ccc(cc1)n2c3c(cn2)c(ncn3)N</t>
-  </si>
-  <si>
-    <t>719540</t>
-  </si>
-  <si>
-    <t>Oc1cc(O)c2c(c1)oc(cc2=O)c1ccccc1</t>
-  </si>
-  <si>
-    <t>[8.416, 10.823]</t>
-  </si>
-  <si>
-    <t>1.7130001783370972</t>
-  </si>
-  <si>
-    <t>254.238</t>
-  </si>
-  <si>
-    <t>1056.0</t>
-  </si>
-  <si>
-    <t>54</t>
-  </si>
-  <si>
-    <t>9</t>
-  </si>
-  <si>
-    <t>c1ccc(cc1)c2cc(=O)c3c(cc(cc3o2)O)O</t>
-  </si>
-  <si>
-    <t>493608</t>
-  </si>
-  <si>
-    <t>COc1cc(C(=O)O)c(cc1OC)Br</t>
-  </si>
-  <si>
-    <t>[3.005]</t>
-  </si>
-  <si>
-    <t>1.7000000476837158</t>
-  </si>
-  <si>
-    <t>261.069</t>
-  </si>
-  <si>
-    <t>10134.0</t>
-  </si>
-  <si>
-    <t>12</t>
-  </si>
-  <si>
-    <t>COc1cc(c(cc1OC)Br)C(=O)O</t>
-  </si>
-  <si>
-    <t>508324</t>
-  </si>
-  <si>
-    <t>Oc1ccc(cc1)n1cnc2c1cccc2</t>
-  </si>
-  <si>
-    <t>[5.82, 8.709]</t>
-  </si>
-  <si>
-    <t>2.2190003395080566</t>
-  </si>
-  <si>
-    <t>210.231</t>
-  </si>
-  <si>
-    <t>21650.2</t>
-  </si>
-  <si>
-    <t>148.0</t>
-  </si>
-  <si>
-    <t>40</t>
-  </si>
-  <si>
-    <t>11</t>
-  </si>
-  <si>
-    <t>c1ccc2c(c1)ncn2c3ccc(cc3)O</t>
-  </si>
-  <si>
-    <t>37095168</t>
-  </si>
-  <si>
-    <t>NC(=O)c1ccc2c(c1)nc([nH]2)c1ccccc1</t>
-  </si>
-  <si>
-    <t>[6.342]</t>
-  </si>
-  <si>
-    <t>2.1920003890991206</t>
-  </si>
-  <si>
-    <t>237.257</t>
-  </si>
-  <si>
-    <t>2000.0</t>
-  </si>
-  <si>
-    <t>42</t>
-  </si>
-  <si>
-    <t>c1ccc(cc1)c2[nH]c3ccc(cc3n2)C(=O)N</t>
-  </si>
-  <si>
-    <t>37053191</t>
-  </si>
-  <si>
-    <t>Nc1ccc2c(c1)ncn2c1ccccc1</t>
-  </si>
-  <si>
-    <t>[6.348]</t>
-  </si>
-  <si>
-    <t>2.3329999446868896</t>
-  </si>
-  <si>
-    <t>209.247</t>
-  </si>
-  <si>
-    <t>50213.0</t>
-  </si>
-  <si>
-    <t>c1ccc(cc1)n2cnc3c2ccc(c3)N</t>
-  </si>
-  <si>
-    <t>31653344</t>
-  </si>
-  <si>
-    <t>O=C(c1c(F)cccc1F)Nc1ccncc1</t>
-  </si>
-  <si>
-    <t>[4.714, 10.538]</t>
-  </si>
-  <si>
-    <t>2.304999828338623</t>
-  </si>
-  <si>
-    <t>234.202</t>
-  </si>
-  <si>
-    <t>100.0</t>
-  </si>
-  <si>
-    <t>c1cc(c(c(c1)F)C(=O)Nc2ccncc2)F</t>
-  </si>
-  <si>
-    <t>2042282</t>
-  </si>
-  <si>
-    <t>O=C(c1n[nH]c2c1cccc2)Nc1ccccc1</t>
-  </si>
-  <si>
-    <t>[8.398]</t>
-  </si>
-  <si>
-    <t>2.6429998874664307</t>
-  </si>
-  <si>
-    <t>762.8</t>
-  </si>
-  <si>
-    <t>13</t>
-  </si>
-  <si>
-    <t>c1ccc(cc1)NC(=O)c2c3ccccc3[nH]n2</t>
-  </si>
-  <si>
-    <t>13419113</t>
-  </si>
-  <si>
-    <t>COc1cc2c(ncnc2cc1OC)Nc1cccc(c1)C</t>
-  </si>
-  <si>
-    <t>[4.267]</t>
-  </si>
-  <si>
-    <t>2.5950002670288086</t>
-  </si>
-  <si>
-    <t>295.336</t>
-  </si>
-  <si>
-    <t>1864.0</t>
-  </si>
-  <si>
-    <t>Cc1cccc(c1)Nc2c3cc(c(cc3ncn2)OC)OC</t>
-  </si>
-  <si>
-    <t>5828805</t>
-  </si>
-  <si>
-    <t>O=C(Nc1nc2c(s1)cccc2)CNC(=O)c1ccccc1</t>
-  </si>
-  <si>
-    <t>[8.672]</t>
-  </si>
-  <si>
-    <t>2.7179999351501465</t>
-  </si>
-  <si>
-    <t>311.358</t>
-  </si>
-  <si>
-    <t>149.1</t>
-  </si>
-  <si>
-    <t>6</t>
-  </si>
-  <si>
-    <t>28</t>
-  </si>
-  <si>
-    <t>14</t>
-  </si>
-  <si>
-    <t>c1ccc(cc1)C(=O)NCC(=O)Nc2nc3ccccc3s2</t>
-  </si>
-  <si>
-    <t>23354217</t>
-  </si>
-  <si>
-    <t>Fc1ccc(cc1)Nc1ncc(c(n1)Nc1ccc(cc1)F)F</t>
-  </si>
-  <si>
-    <t>[3.892]</t>
-  </si>
-  <si>
-    <t>2.813999652862549</t>
-  </si>
-  <si>
-    <t>316.281</t>
-  </si>
-  <si>
-    <t>105.0</t>
-  </si>
-  <si>
-    <t>c1cc(ccc1Nc2c(cnc(n2)Nc3ccc(cc3)F)F)F</t>
-  </si>
-  <si>
-    <t>1698122</t>
-  </si>
-  <si>
-    <t>Brc1cncc(c1)C(=O)Nc1cccc2c1nccc2</t>
-  </si>
-  <si>
-    <t>[4.001, 10.328]</t>
-  </si>
-  <si>
-    <t>2.922999620437622</t>
-  </si>
-  <si>
-    <t>328.163</t>
-  </si>
-  <si>
-    <t>406.0</t>
-  </si>
-  <si>
-    <t>37</t>
-  </si>
-  <si>
-    <t>15</t>
-  </si>
-  <si>
-    <t>c1cc2cccnc2c(c1)NC(=O)c3cc(cnc3)Br</t>
-  </si>
-  <si>
-    <t>18893169</t>
-  </si>
-  <si>
-    <t>COc1cccc(c1)Nc1ncnc2c1cccc2.Cl</t>
-  </si>
-  <si>
-    <t>[4.05]</t>
-  </si>
-  <si>
-    <t>3.138999938964844</t>
-  </si>
-  <si>
-    <t>287.744</t>
-  </si>
-  <si>
-    <t>119.7</t>
-  </si>
-  <si>
-    <t>16</t>
-  </si>
-  <si>
-    <t>COc1cccc(c1)Nc2c3ccccc3ncn2.Cl</t>
-  </si>
-  <si>
-    <t>1865544</t>
-  </si>
-  <si>
-    <t>c1ccc(cc1)CSc1nnc(o1)c1ccncc1</t>
-  </si>
-  <si>
-    <t>[4.902]</t>
-  </si>
-  <si>
-    <t>3.3059999942779537</t>
-  </si>
-  <si>
-    <t>269.322</t>
-  </si>
-  <si>
-    <t>170.0</t>
-  </si>
-  <si>
-    <t>30</t>
-  </si>
-  <si>
-    <t>17</t>
-  </si>
-  <si>
-    <t>c1ccc(cc1)CSc2nnc(o2)c3ccncc3</t>
-  </si>
-  <si>
-    <t>1444229</t>
-  </si>
-  <si>
-    <t>O=C(c1cccs1)Nc1nnc(s1)Cc1ccccc1</t>
-  </si>
-  <si>
-    <t>[7.12]</t>
-  </si>
-  <si>
-    <t>3.6050002574920654</t>
-  </si>
-  <si>
-    <t>301.387</t>
-  </si>
-  <si>
-    <t>379.0</t>
-  </si>
-  <si>
-    <t>18</t>
-  </si>
-  <si>
-    <t>c1ccc(cc1)Cc2nnc(s2)NC(=O)c3cccs3</t>
-  </si>
-  <si>
-    <t>1228629</t>
-  </si>
-  <si>
-    <t>Clc1ccc(o1)C(=O)Nc1ccccc1N1CCCCC1</t>
-  </si>
-  <si>
-    <t>[5.346]</t>
-  </si>
-  <si>
-    <t>3.794999837875366</t>
-  </si>
-  <si>
-    <t>304.771</t>
-  </si>
-  <si>
-    <t>424.3</t>
-  </si>
-  <si>
-    <t>19</t>
-  </si>
-  <si>
-    <t>c1ccc(c(c1)NC(=O)c2ccc(o2)Cl)N3CCCCC3</t>
-  </si>
-  <si>
-    <t>18908671</t>
-  </si>
-  <si>
-    <t>O=C1S/C(=C/c2ccc(o2)c2ccc(c(c2)Cl)F)/C(=O)N1</t>
-  </si>
-  <si>
-    <t>[8.052]</t>
-  </si>
-  <si>
-    <t>3.9079997539520255</t>
-  </si>
-  <si>
-    <t>323.7270000000001</t>
-  </si>
-  <si>
-    <t>125.0</t>
-  </si>
-  <si>
-    <t>c1cc(c(cc1c2ccc(o2)/C=C/3\C(=O)NC(=O)S3)Cl)F</t>
-  </si>
-  <si>
-    <t>25775231</t>
-  </si>
-  <si>
-    <t>FC(c1ccc(cc1)c1nnc2n1nc(cc2)NC1CC1)(F)F</t>
-  </si>
-  <si>
-    <t>[4.394]</t>
-  </si>
-  <si>
-    <t>4.128999710083009</t>
-  </si>
-  <si>
-    <t>319.284</t>
-  </si>
-  <si>
-    <t>3175.0</t>
-  </si>
-  <si>
-    <t>32</t>
-  </si>
-  <si>
-    <t>21</t>
-  </si>
-  <si>
-    <t>c1cc(ccc1c2nnc3n2nc(cc3)NC4CC4)C(F)(F)F</t>
-  </si>
-  <si>
-    <t>5784088</t>
-  </si>
-  <si>
-    <t>O=C1Nc2c(/C/1=C/c1ccc(cc1)C(C)C)cccc2</t>
-  </si>
-  <si>
-    <t>[3.158]</t>
-  </si>
-  <si>
-    <t>4.2330002784728995</t>
-  </si>
-  <si>
-    <t>263.334</t>
-  </si>
-  <si>
-    <t>283.7</t>
-  </si>
-  <si>
-    <t>24</t>
-  </si>
-  <si>
     <t>22</t>
   </si>
   <si>
@@ -698,33 +713,6 @@
   </si>
   <si>
     <t>45809595</t>
-  </si>
-  <si>
-    <t>CCOC(=O)c1c(=O)[nH]c2c(c1c1ccccc1)cc(cc2)Cl</t>
-  </si>
-  <si>
-    <t>[8.549]</t>
-  </si>
-  <si>
-    <t>4.517000198364258</t>
-  </si>
-  <si>
-    <t>327.76199999999994</t>
-  </si>
-  <si>
-    <t>1059.0</t>
-  </si>
-  <si>
-    <t>59</t>
-  </si>
-  <si>
-    <t>23</t>
-  </si>
-  <si>
-    <t>CCOC(=O)c1c(c2cc(ccc2[nH]c1=O)Cl)c3ccccc3</t>
-  </si>
-  <si>
-    <t>703997</t>
   </si>
 </sst>
 </file>
@@ -2179,248 +2167,248 @@
         <v>26</v>
       </c>
       <c r="L3" s="2" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="M3" s="2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="N3" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="O3" s="2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="P3" s="2" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="4" spans="1:16" s="3" customFormat="1" ht="187.5" customHeight="1">
       <c r="B4" s="3" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="H4" s="3" t="s">
         <v>23</v>
       </c>
       <c r="I4" s="3" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="J4" s="3" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="K4" s="3" t="s">
         <v>26</v>
       </c>
       <c r="L4" s="3" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="M4" s="3" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="N4" s="3" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="O4" s="3" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="P4" s="3" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="5" spans="1:16" s="2" customFormat="1" ht="187.5" customHeight="1">
       <c r="B5" s="2" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="H5" s="2" t="s">
         <v>23</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>38</v>
+        <v>48</v>
       </c>
       <c r="J5" s="2" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="K5" s="2" t="s">
         <v>26</v>
       </c>
       <c r="L5" s="2" t="s">
-        <v>38</v>
+        <v>50</v>
       </c>
       <c r="M5" s="2" t="s">
-        <v>48</v>
+        <v>28</v>
       </c>
       <c r="N5" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="O5" s="2" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="P5" s="2" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
     </row>
     <row r="6" spans="1:16" s="3" customFormat="1" ht="187.5" customHeight="1">
       <c r="B6" s="3" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>36</v>
+        <v>58</v>
       </c>
       <c r="H6" s="3" t="s">
         <v>23</v>
       </c>
       <c r="I6" s="3" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="J6" s="3" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="K6" s="3" t="s">
         <v>26</v>
       </c>
       <c r="L6" s="3" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
       <c r="M6" s="3" t="s">
-        <v>27</v>
+        <v>59</v>
       </c>
       <c r="N6" s="3" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="O6" s="3" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="P6" s="3" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
     </row>
     <row r="7" spans="1:16" s="2" customFormat="1" ht="187.5" customHeight="1">
       <c r="B7" s="2" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="H7" s="2" t="s">
         <v>23</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="J7" s="2" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="K7" s="2" t="s">
         <v>26</v>
       </c>
       <c r="L7" s="2" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="M7" s="2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="N7" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="O7" s="2" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="P7" s="2" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
     </row>
     <row r="8" spans="1:16" s="3" customFormat="1" ht="187.5" customHeight="1">
       <c r="B8" s="3" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>76</v>
+        <v>47</v>
       </c>
       <c r="H8" s="3" t="s">
         <v>23</v>
       </c>
       <c r="I8" s="3" t="s">
-        <v>27</v>
+        <v>59</v>
       </c>
       <c r="J8" s="3" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="K8" s="3" t="s">
         <v>26</v>
       </c>
       <c r="L8" s="3" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="M8" s="3" t="s">
-        <v>27</v>
+        <v>59</v>
       </c>
       <c r="N8" s="3" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="O8" s="3" t="s">
         <v>79</v>
@@ -2446,216 +2434,216 @@
         <v>85</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>36</v>
+        <v>68</v>
       </c>
       <c r="H9" s="2" t="s">
         <v>23</v>
       </c>
       <c r="I9" s="2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="J9" s="2" t="s">
-        <v>86</v>
+        <v>69</v>
       </c>
       <c r="K9" s="2" t="s">
         <v>26</v>
       </c>
       <c r="L9" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="M9" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="N9" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="O9" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="P9" s="2" t="s">
         <v>87</v>
-      </c>
-      <c r="M9" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="N9" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="O9" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="P9" s="2" t="s">
-        <v>89</v>
       </c>
     </row>
     <row r="10" spans="1:16" s="3" customFormat="1" ht="187.5" customHeight="1">
       <c r="B10" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="D10" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="C10" s="3" t="s">
+      <c r="E10" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="D10" s="3" t="s">
+      <c r="F10" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="E10" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="F10" s="3" t="s">
-        <v>94</v>
-      </c>
       <c r="G10" s="3" t="s">
-        <v>36</v>
+        <v>47</v>
       </c>
       <c r="H10" s="3" t="s">
         <v>23</v>
       </c>
       <c r="I10" s="3" t="s">
-        <v>24</v>
+        <v>48</v>
       </c>
       <c r="J10" s="3" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="K10" s="3" t="s">
         <v>26</v>
       </c>
       <c r="L10" s="3" t="s">
-        <v>87</v>
+        <v>60</v>
       </c>
       <c r="M10" s="3" t="s">
-        <v>48</v>
+        <v>59</v>
       </c>
       <c r="N10" s="3" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="O10" s="3" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="P10" s="3" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="11" spans="1:16" s="2" customFormat="1" ht="187.5" customHeight="1">
       <c r="B11" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="D11" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="C11" s="2" t="s">
+      <c r="E11" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="F11" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="D11" s="2" t="s">
+      <c r="G11" s="2" t="s">
         <v>100</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="F11" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="G11" s="2" t="s">
-        <v>103</v>
       </c>
       <c r="H11" s="2" t="s">
         <v>23</v>
       </c>
       <c r="I11" s="2" t="s">
-        <v>27</v>
+        <v>48</v>
       </c>
       <c r="J11" s="2" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="K11" s="2" t="s">
         <v>26</v>
       </c>
       <c r="L11" s="2" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="M11" s="2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="N11" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="O11" s="2" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="P11" s="2" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
     </row>
     <row r="12" spans="1:16" s="3" customFormat="1" ht="187.5" customHeight="1">
       <c r="B12" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="E12" s="3" t="s">
         <v>108</v>
       </c>
-      <c r="C12" s="3" t="s">
+      <c r="F12" s="3" t="s">
         <v>109</v>
       </c>
-      <c r="D12" s="3" t="s">
+      <c r="G12" s="3" t="s">
         <v>110</v>
-      </c>
-      <c r="E12" s="3" t="s">
-        <v>111</v>
-      </c>
-      <c r="F12" s="3" t="s">
-        <v>112</v>
-      </c>
-      <c r="G12" s="3" t="s">
-        <v>36</v>
       </c>
       <c r="H12" s="3" t="s">
         <v>23</v>
       </c>
       <c r="I12" s="3" t="s">
-        <v>48</v>
+        <v>28</v>
       </c>
       <c r="J12" s="3" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="K12" s="3" t="s">
         <v>26</v>
       </c>
       <c r="L12" s="3" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="M12" s="3" t="s">
-        <v>48</v>
+        <v>59</v>
       </c>
       <c r="N12" s="3" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="O12" s="3" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="P12" s="3" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="13" spans="1:16" s="2" customFormat="1" ht="187.5" customHeight="1">
       <c r="B13" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="D13" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="C13" s="2" t="s">
+      <c r="E13" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="D13" s="2" t="s">
+      <c r="F13" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="E13" s="2" t="s">
-        <v>119</v>
-      </c>
-      <c r="F13" s="2" t="s">
-        <v>120</v>
-      </c>
       <c r="G13" s="2" t="s">
-        <v>103</v>
+        <v>68</v>
       </c>
       <c r="H13" s="2" t="s">
         <v>23</v>
       </c>
       <c r="I13" s="2" t="s">
-        <v>27</v>
+        <v>119</v>
       </c>
       <c r="J13" s="2" t="s">
-        <v>104</v>
+        <v>93</v>
       </c>
       <c r="K13" s="2" t="s">
         <v>26</v>
       </c>
       <c r="L13" s="2" t="s">
-        <v>95</v>
+        <v>120</v>
       </c>
       <c r="M13" s="2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="N13" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="O13" s="2" t="s">
         <v>121</v>
@@ -2681,28 +2669,28 @@
         <v>127</v>
       </c>
       <c r="G14" s="3" t="s">
-        <v>36</v>
+        <v>47</v>
       </c>
       <c r="H14" s="3" t="s">
         <v>23</v>
       </c>
       <c r="I14" s="3" t="s">
-        <v>24</v>
+        <v>48</v>
       </c>
       <c r="J14" s="3" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="K14" s="3" t="s">
         <v>26</v>
       </c>
       <c r="L14" s="3" t="s">
-        <v>95</v>
+        <v>120</v>
       </c>
       <c r="M14" s="3" t="s">
-        <v>48</v>
+        <v>59</v>
       </c>
       <c r="N14" s="3" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="O14" s="3" t="s">
         <v>128</v>
@@ -2722,116 +2710,116 @@
         <v>132</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>111</v>
+        <v>133</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>22</v>
+        <v>68</v>
       </c>
       <c r="H15" s="2" t="s">
         <v>23</v>
       </c>
       <c r="I15" s="2" t="s">
-        <v>24</v>
+        <v>48</v>
       </c>
       <c r="J15" s="2" t="s">
-        <v>67</v>
+        <v>135</v>
       </c>
       <c r="K15" s="2" t="s">
         <v>26</v>
       </c>
       <c r="L15" s="2" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="M15" s="2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="N15" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="O15" s="2" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="P15" s="2" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
     </row>
     <row r="16" spans="1:16" s="3" customFormat="1" ht="187.5" customHeight="1">
       <c r="B16" s="3" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="G16" s="3" t="s">
-        <v>76</v>
+        <v>47</v>
       </c>
       <c r="H16" s="3" t="s">
         <v>23</v>
       </c>
       <c r="I16" s="3" t="s">
-        <v>38</v>
+        <v>48</v>
       </c>
       <c r="J16" s="3" t="s">
-        <v>67</v>
+        <v>49</v>
       </c>
       <c r="K16" s="3" t="s">
         <v>26</v>
       </c>
       <c r="L16" s="3" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="M16" s="3" t="s">
-        <v>48</v>
+        <v>59</v>
       </c>
       <c r="N16" s="3" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="O16" s="3" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="P16" s="3" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
     </row>
     <row r="17" spans="2:16" s="2" customFormat="1" ht="187.5" customHeight="1">
       <c r="B17" s="2" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>103</v>
+        <v>68</v>
       </c>
       <c r="H17" s="2" t="s">
         <v>23</v>
       </c>
       <c r="I17" s="2" t="s">
-        <v>149</v>
+        <v>48</v>
       </c>
       <c r="J17" s="2" t="s">
-        <v>150</v>
+        <v>101</v>
       </c>
       <c r="K17" s="2" t="s">
         <v>26</v>
@@ -2840,10 +2828,10 @@
         <v>151</v>
       </c>
       <c r="M17" s="2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="N17" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="O17" s="2" t="s">
         <v>152</v>
@@ -2869,16 +2857,16 @@
         <v>158</v>
       </c>
       <c r="G18" s="3" t="s">
-        <v>36</v>
+        <v>47</v>
       </c>
       <c r="H18" s="3" t="s">
         <v>23</v>
       </c>
       <c r="I18" s="3" t="s">
-        <v>38</v>
+        <v>28</v>
       </c>
       <c r="J18" s="3" t="s">
-        <v>150</v>
+        <v>69</v>
       </c>
       <c r="K18" s="3" t="s">
         <v>26</v>
@@ -2887,10 +2875,10 @@
         <v>151</v>
       </c>
       <c r="M18" s="3" t="s">
-        <v>48</v>
+        <v>59</v>
       </c>
       <c r="N18" s="3" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="O18" s="3" t="s">
         <v>159</v>
@@ -2916,13 +2904,13 @@
         <v>165</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>103</v>
+        <v>47</v>
       </c>
       <c r="H19" s="2" t="s">
         <v>23</v>
       </c>
       <c r="I19" s="2" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="J19" s="2" t="s">
         <v>166</v>
@@ -2934,10 +2922,10 @@
         <v>167</v>
       </c>
       <c r="M19" s="2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="N19" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="O19" s="2" t="s">
         <v>168</v>
@@ -2963,28 +2951,28 @@
         <v>174</v>
       </c>
       <c r="G20" s="3" t="s">
-        <v>103</v>
+        <v>47</v>
       </c>
       <c r="H20" s="3" t="s">
         <v>23</v>
       </c>
       <c r="I20" s="3" t="s">
-        <v>24</v>
+        <v>119</v>
       </c>
       <c r="J20" s="3" t="s">
-        <v>67</v>
+        <v>175</v>
       </c>
       <c r="K20" s="3" t="s">
         <v>26</v>
       </c>
       <c r="L20" s="3" t="s">
-        <v>175</v>
+        <v>167</v>
       </c>
       <c r="M20" s="3" t="s">
-        <v>27</v>
+        <v>59</v>
       </c>
       <c r="N20" s="3" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="O20" s="3" t="s">
         <v>176</v>
@@ -3010,16 +2998,16 @@
         <v>182</v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>36</v>
+        <v>68</v>
       </c>
       <c r="H21" s="2" t="s">
         <v>23</v>
       </c>
       <c r="I21" s="2" t="s">
-        <v>38</v>
+        <v>183</v>
       </c>
       <c r="J21" s="2" t="s">
-        <v>183</v>
+        <v>120</v>
       </c>
       <c r="K21" s="2" t="s">
         <v>26</v>
@@ -3028,10 +3016,10 @@
         <v>184</v>
       </c>
       <c r="M21" s="2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="N21" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="O21" s="2" t="s">
         <v>185</v>
@@ -3057,269 +3045,269 @@
         <v>191</v>
       </c>
       <c r="G22" s="3" t="s">
-        <v>103</v>
+        <v>68</v>
       </c>
       <c r="H22" s="3" t="s">
         <v>23</v>
       </c>
       <c r="I22" s="3" t="s">
-        <v>58</v>
+        <v>48</v>
       </c>
       <c r="J22" s="3" t="s">
-        <v>151</v>
+        <v>101</v>
       </c>
       <c r="K22" s="3" t="s">
         <v>26</v>
       </c>
       <c r="L22" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="M22" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="N22" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="O22" s="3" t="s">
         <v>192</v>
       </c>
-      <c r="M22" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="N22" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="O22" s="3" t="s">
+      <c r="P22" s="3" t="s">
         <v>193</v>
-      </c>
-      <c r="P22" s="3" t="s">
-        <v>194</v>
       </c>
     </row>
     <row r="23" spans="2:16" s="2" customFormat="1" ht="187.5" customHeight="1">
       <c r="B23" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="C23" s="2" t="s">
         <v>195</v>
       </c>
-      <c r="C23" s="2" t="s">
+      <c r="D23" s="2" t="s">
         <v>196</v>
       </c>
-      <c r="D23" s="2" t="s">
+      <c r="E23" s="2" t="s">
         <v>197</v>
       </c>
-      <c r="E23" s="2" t="s">
+      <c r="F23" s="2" t="s">
         <v>198</v>
       </c>
-      <c r="F23" s="2" t="s">
-        <v>199</v>
-      </c>
       <c r="G23" s="2" t="s">
-        <v>103</v>
+        <v>68</v>
       </c>
       <c r="H23" s="2" t="s">
         <v>23</v>
       </c>
       <c r="I23" s="2" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
       <c r="J23" s="2" t="s">
-        <v>192</v>
+        <v>184</v>
       </c>
       <c r="K23" s="2" t="s">
         <v>26</v>
       </c>
       <c r="L23" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="M23" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="N23" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="O23" s="2" t="s">
+        <v>199</v>
+      </c>
+      <c r="P23" s="2" t="s">
         <v>200</v>
-      </c>
-      <c r="M23" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="N23" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="O23" s="2" t="s">
-        <v>201</v>
-      </c>
-      <c r="P23" s="2" t="s">
-        <v>202</v>
       </c>
     </row>
     <row r="24" spans="2:16" s="3" customFormat="1" ht="187.5" customHeight="1">
       <c r="B24" s="3" t="s">
+        <v>201</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>202</v>
+      </c>
+      <c r="D24" s="3" t="s">
         <v>203</v>
       </c>
-      <c r="C24" s="3" t="s">
+      <c r="E24" s="3" t="s">
         <v>204</v>
       </c>
-      <c r="D24" s="3" t="s">
+      <c r="F24" s="3" t="s">
         <v>205</v>
       </c>
-      <c r="E24" s="3" t="s">
-        <v>206</v>
-      </c>
-      <c r="F24" s="3" t="s">
-        <v>207</v>
-      </c>
       <c r="G24" s="3" t="s">
-        <v>36</v>
+        <v>47</v>
       </c>
       <c r="H24" s="3" t="s">
         <v>23</v>
       </c>
       <c r="I24" s="3" t="s">
-        <v>48</v>
+        <v>27</v>
       </c>
       <c r="J24" s="3" t="s">
-        <v>77</v>
+        <v>206</v>
       </c>
       <c r="K24" s="3" t="s">
         <v>26</v>
       </c>
       <c r="L24" s="3" t="s">
-        <v>47</v>
+        <v>111</v>
       </c>
       <c r="M24" s="3" t="s">
-        <v>27</v>
+        <v>59</v>
       </c>
       <c r="N24" s="3" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="O24" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="P24" s="3" t="s">
         <v>208</v>
-      </c>
-      <c r="P24" s="3" t="s">
-        <v>209</v>
       </c>
     </row>
     <row r="25" spans="2:16" s="2" customFormat="1" ht="187.5" customHeight="1">
       <c r="B25" s="2" t="s">
+        <v>209</v>
+      </c>
+      <c r="C25" s="2" t="s">
         <v>210</v>
       </c>
-      <c r="C25" s="2" t="s">
+      <c r="D25" s="2" t="s">
         <v>211</v>
       </c>
-      <c r="D25" s="2" t="s">
+      <c r="E25" s="2" t="s">
         <v>212</v>
       </c>
-      <c r="E25" s="2" t="s">
+      <c r="F25" s="2" t="s">
         <v>213</v>
       </c>
-      <c r="F25" s="2" t="s">
-        <v>214</v>
-      </c>
       <c r="G25" s="2" t="s">
-        <v>76</v>
+        <v>47</v>
       </c>
       <c r="H25" s="2" t="s">
         <v>23</v>
       </c>
       <c r="I25" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="J25" s="2" t="s">
         <v>38</v>
-      </c>
-      <c r="J25" s="2" t="s">
-        <v>215</v>
       </c>
       <c r="K25" s="2" t="s">
         <v>26</v>
       </c>
       <c r="L25" s="2" t="s">
-        <v>216</v>
+        <v>49</v>
       </c>
       <c r="M25" s="2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="N25" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="O25" s="2" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="P25" s="2" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
     </row>
     <row r="26" spans="2:16" s="3" customFormat="1" ht="187.5" customHeight="1">
       <c r="B26" s="3" t="s">
+        <v>216</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>217</v>
+      </c>
+      <c r="D26" s="3" t="s">
+        <v>218</v>
+      </c>
+      <c r="E26" s="3" t="s">
         <v>219</v>
       </c>
-      <c r="C26" s="3" t="s">
+      <c r="F26" s="3" t="s">
         <v>220</v>
       </c>
-      <c r="D26" s="3" t="s">
-        <v>221</v>
-      </c>
-      <c r="E26" s="3" t="s">
-        <v>222</v>
-      </c>
-      <c r="F26" s="3" t="s">
-        <v>223</v>
-      </c>
       <c r="G26" s="3" t="s">
-        <v>66</v>
+        <v>37</v>
       </c>
       <c r="H26" s="3" t="s">
         <v>23</v>
       </c>
       <c r="I26" s="3" t="s">
-        <v>48</v>
+        <v>27</v>
       </c>
       <c r="J26" s="3" t="s">
-        <v>224</v>
+        <v>175</v>
       </c>
       <c r="K26" s="3" t="s">
         <v>26</v>
       </c>
       <c r="L26" s="3" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
       <c r="M26" s="3" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="N26" s="3" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="O26" s="3" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="P26" s="3" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
     </row>
     <row r="27" spans="2:16" s="2" customFormat="1" ht="187.5" customHeight="1">
       <c r="B27" s="2" t="s">
+        <v>224</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="E27" s="2" t="s">
+        <v>227</v>
+      </c>
+      <c r="F27" s="2" t="s">
         <v>228</v>
       </c>
-      <c r="C27" s="2" t="s">
+      <c r="G27" s="2" t="s">
         <v>229</v>
-      </c>
-      <c r="D27" s="2" t="s">
-        <v>230</v>
-      </c>
-      <c r="E27" s="2" t="s">
-        <v>231</v>
-      </c>
-      <c r="F27" s="2" t="s">
-        <v>232</v>
-      </c>
-      <c r="G27" s="2" t="s">
-        <v>36</v>
       </c>
       <c r="H27" s="2" t="s">
         <v>23</v>
       </c>
       <c r="I27" s="2" t="s">
-        <v>38</v>
+        <v>59</v>
       </c>
       <c r="J27" s="2" t="s">
-        <v>233</v>
+        <v>206</v>
       </c>
       <c r="K27" s="2" t="s">
         <v>26</v>
       </c>
       <c r="L27" s="2" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="M27" s="2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="N27" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="O27" s="2" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="P27" s="2" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Round2: Filter compounds with Chemspider logPs.
</commit_message>
<xml_diff>
--- a/compound_selection/zinc15_eMolecules_intersection_set/20170807_zinc15_eMolecules_subset_depiction/df_frag_final_oe.xlsx
+++ b/compound_selection/zinc15_eMolecules_intersection_set/20170807_zinc15_eMolecules_subset_depiction/df_frag_final_oe.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="392" uniqueCount="233">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="392" uniqueCount="230">
   <si>
     <t>df_frag_final_oe.csv</t>
   </si>
@@ -142,541 +142,532 @@
     <t>719540</t>
   </si>
   <si>
-    <t>O=C(c1ccccc1)Nc1ccncc1</t>
-  </si>
-  <si>
-    <t>[4.714]</t>
-  </si>
-  <si>
-    <t>1.694999933242798</t>
-  </si>
-  <si>
-    <t>198.221</t>
-  </si>
-  <si>
-    <t>116.0</t>
+    <t>Oc1ccc(cc1)n1cnc2c1cccc2</t>
+  </si>
+  <si>
+    <t>[5.82, 8.709]</t>
+  </si>
+  <si>
+    <t>2.2190003395080566</t>
+  </si>
+  <si>
+    <t>210.231</t>
+  </si>
+  <si>
+    <t>21650.2</t>
+  </si>
+  <si>
+    <t>148.0</t>
+  </si>
+  <si>
+    <t>40</t>
+  </si>
+  <si>
+    <t>11</t>
+  </si>
+  <si>
+    <t>c1ccc2c(c1)ncn2c3ccc(cc3)O</t>
+  </si>
+  <si>
+    <t>37095168</t>
+  </si>
+  <si>
+    <t>NC(=O)c1ccc2c(c1)nc([nH]2)c1ccccc1</t>
+  </si>
+  <si>
+    <t>[6.342]</t>
+  </si>
+  <si>
+    <t>2.1920003890991206</t>
+  </si>
+  <si>
+    <t>237.257</t>
+  </si>
+  <si>
+    <t>2000.0</t>
   </si>
   <si>
     <t>168.0</t>
   </si>
   <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>42</t>
+  </si>
+  <si>
+    <t>c1ccc(cc1)c2[nH]c3ccc(cc3n2)C(=O)N</t>
+  </si>
+  <si>
+    <t>37053191</t>
+  </si>
+  <si>
+    <t>CCn1c(nc2c1cccc2)c1nonc1N</t>
+  </si>
+  <si>
+    <t>[4.082]</t>
+  </si>
+  <si>
+    <t>2.068000078201294</t>
+  </si>
+  <si>
+    <t>229.238</t>
+  </si>
+  <si>
+    <t>385.3</t>
+  </si>
+  <si>
+    <t>223.0</t>
+  </si>
+  <si>
+    <t>28</t>
+  </si>
+  <si>
     <t>3</t>
   </si>
   <si>
+    <t>CCn1c2ccccc2nc1c3c(non3)N</t>
+  </si>
+  <si>
+    <t>1360661</t>
+  </si>
+  <si>
+    <t>Nc1ccc2c(c1)ncn2c1ccccc1</t>
+  </si>
+  <si>
+    <t>[6.348]</t>
+  </si>
+  <si>
+    <t>2.3329999446868896</t>
+  </si>
+  <si>
+    <t>209.247</t>
+  </si>
+  <si>
+    <t>50213.0</t>
+  </si>
+  <si>
+    <t>12</t>
+  </si>
+  <si>
+    <t>c1ccc(cc1)n2cnc3c2ccc(c3)N</t>
+  </si>
+  <si>
+    <t>31653344</t>
+  </si>
+  <si>
+    <t>Nc1nonc1c1nc2c(n1CC1CC1)cccc2</t>
+  </si>
+  <si>
+    <t>2.43999981880188</t>
+  </si>
+  <si>
+    <t>255.275</t>
+  </si>
+  <si>
+    <t>300.0</t>
+  </si>
+  <si>
+    <t>c1ccc2c(c1)nc(n2CC3CC3)c4c(non4)N</t>
+  </si>
+  <si>
+    <t>8332960</t>
+  </si>
+  <si>
+    <t>O=C(c1n[nH]c2c1cccc2)Nc1ccccc1</t>
+  </si>
+  <si>
+    <t>[8.398]</t>
+  </si>
+  <si>
+    <t>2.6429998874664307</t>
+  </si>
+  <si>
+    <t>762.8</t>
+  </si>
+  <si>
+    <t>36</t>
+  </si>
+  <si>
+    <t>13</t>
+  </si>
+  <si>
+    <t>c1ccc(cc1)NC(=O)c2c3ccccc3[nH]n2</t>
+  </si>
+  <si>
+    <t>13419113</t>
+  </si>
+  <si>
+    <t>COc1cc2c(ncnc2cc1OC)Nc1cccc(c1)C</t>
+  </si>
+  <si>
+    <t>[4.267]</t>
+  </si>
+  <si>
+    <t>2.5950002670288086</t>
+  </si>
+  <si>
+    <t>295.336</t>
+  </si>
+  <si>
+    <t>1864.0</t>
+  </si>
+  <si>
+    <t>Cc1cccc(c1)Nc2c3cc(c(cc3ncn2)OC)OC</t>
+  </si>
+  <si>
+    <t>5828805</t>
+  </si>
+  <si>
+    <t>O=C(Nc1nc2c(s1)cccc2)CNC(=O)c1ccccc1</t>
+  </si>
+  <si>
+    <t>[8.672]</t>
+  </si>
+  <si>
+    <t>2.7179999351501465</t>
+  </si>
+  <si>
+    <t>311.358</t>
+  </si>
+  <si>
+    <t>149.1</t>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
+    <t>14</t>
+  </si>
+  <si>
+    <t>c1ccc(cc1)C(=O)NCC(=O)Nc2nc3ccccc3s2</t>
+  </si>
+  <si>
+    <t>23354217</t>
+  </si>
+  <si>
+    <t>OC(=O)Cc1c(=O)[nH]c2c(c1c1ccccc1)cc(cc2)C</t>
+  </si>
+  <si>
+    <t>[4.109]</t>
+  </si>
+  <si>
+    <t>2.8030002117156982</t>
+  </si>
+  <si>
+    <t>293.317</t>
+  </si>
+  <si>
+    <t>232.1</t>
+  </si>
+  <si>
+    <t>59</t>
+  </si>
+  <si>
+    <t>Cc1ccc2c(c1)c(c(c(=O)[nH]2)CC(=O)O)c3ccccc3</t>
+  </si>
+  <si>
+    <t>1367649</t>
+  </si>
+  <si>
+    <t>Brc1cncc(c1)C(=O)Nc1cccc2c1nccc2</t>
+  </si>
+  <si>
+    <t>[4.001, 10.328]</t>
+  </si>
+  <si>
+    <t>2.922999620437622</t>
+  </si>
+  <si>
+    <t>328.163</t>
+  </si>
+  <si>
+    <t>406.0</t>
+  </si>
+  <si>
+    <t>37</t>
+  </si>
+  <si>
+    <t>15</t>
+  </si>
+  <si>
+    <t>c1cc2cccnc2c(c1)NC(=O)c3cc(cnc3)Br</t>
+  </si>
+  <si>
+    <t>18893169</t>
+  </si>
+  <si>
+    <t>O=C(c1ccncc1)Nc1c(Cl)cccc1Cl</t>
+  </si>
+  <si>
+    <t>[3.163, 9.847]</t>
+  </si>
+  <si>
+    <t>2.9270000457763667</t>
+  </si>
+  <si>
+    <t>267.111</t>
+  </si>
+  <si>
+    <t>109.0</t>
+  </si>
+  <si>
     <t>20</t>
   </si>
   <si>
-    <t>9</t>
-  </si>
-  <si>
-    <t>c1ccc(cc1)C(=O)Nc2ccncc2</t>
-  </si>
-  <si>
-    <t>45490344</t>
-  </si>
-  <si>
-    <t>CSc1ccc(cc1)/C=C\1/NC(=O)NC1=O</t>
-  </si>
-  <si>
-    <t>[8.74]</t>
-  </si>
-  <si>
-    <t>1.8569998741149905</t>
-  </si>
-  <si>
-    <t>234.274</t>
-  </si>
-  <si>
-    <t>135.0</t>
-  </si>
-  <si>
-    <t>355.0</t>
-  </si>
-  <si>
-    <t>2</t>
-  </si>
-  <si>
-    <t>12</t>
-  </si>
-  <si>
-    <t>CSc1ccc(cc1)/C=C/2\C(=O)NC(=O)N2</t>
-  </si>
-  <si>
-    <t>27013168</t>
-  </si>
-  <si>
-    <t>Oc1ccc(cc1)n1cnc2c1cccc2</t>
-  </si>
-  <si>
-    <t>[5.82, 8.709]</t>
-  </si>
-  <si>
-    <t>2.2190003395080566</t>
-  </si>
-  <si>
-    <t>210.231</t>
-  </si>
-  <si>
-    <t>21650.2</t>
-  </si>
-  <si>
-    <t>148.0</t>
-  </si>
-  <si>
-    <t>40</t>
-  </si>
-  <si>
-    <t>11</t>
-  </si>
-  <si>
-    <t>c1ccc2c(c1)ncn2c3ccc(cc3)O</t>
-  </si>
-  <si>
-    <t>37095168</t>
-  </si>
-  <si>
-    <t>NC(=O)c1ccc2c(c1)nc([nH]2)c1ccccc1</t>
-  </si>
-  <si>
-    <t>[6.342]</t>
-  </si>
-  <si>
-    <t>2.1920003890991206</t>
-  </si>
-  <si>
-    <t>237.257</t>
-  </si>
-  <si>
-    <t>2000.0</t>
-  </si>
-  <si>
-    <t>42</t>
-  </si>
-  <si>
-    <t>c1ccc(cc1)c2[nH]c3ccc(cc3n2)C(=O)N</t>
-  </si>
-  <si>
-    <t>37053191</t>
-  </si>
-  <si>
-    <t>Nc1ccc2c(c1)ncn2c1ccccc1</t>
-  </si>
-  <si>
-    <t>[6.348]</t>
-  </si>
-  <si>
-    <t>2.3329999446868896</t>
-  </si>
-  <si>
-    <t>209.247</t>
-  </si>
-  <si>
-    <t>50213.0</t>
-  </si>
-  <si>
-    <t>c1ccc(cc1)n2cnc3c2ccc(c3)N</t>
-  </si>
-  <si>
-    <t>31653344</t>
-  </si>
-  <si>
-    <t>Nc1nonc1c1nc2c(n1CC1CC1)cccc2</t>
-  </si>
-  <si>
-    <t>[4.082]</t>
-  </si>
-  <si>
-    <t>2.43999981880188</t>
-  </si>
-  <si>
-    <t>255.275</t>
-  </si>
-  <si>
-    <t>300.0</t>
-  </si>
-  <si>
-    <t>28</t>
-  </si>
-  <si>
-    <t>c1ccc2c(c1)nc(n2CC3CC3)c4c(non4)N</t>
-  </si>
-  <si>
-    <t>8332960</t>
-  </si>
-  <si>
-    <t>O=C(c1n[nH]c2c1cccc2)Nc1ccccc1</t>
-  </si>
-  <si>
-    <t>[8.398]</t>
-  </si>
-  <si>
-    <t>2.6429998874664307</t>
-  </si>
-  <si>
-    <t>762.8</t>
-  </si>
-  <si>
-    <t>223.0</t>
-  </si>
-  <si>
-    <t>36</t>
-  </si>
-  <si>
-    <t>13</t>
-  </si>
-  <si>
-    <t>c1ccc(cc1)NC(=O)c2c3ccccc3[nH]n2</t>
-  </si>
-  <si>
-    <t>13419113</t>
-  </si>
-  <si>
-    <t>Nc1ccc(cc1)c1nn2c(s1)nnc2C</t>
-  </si>
-  <si>
-    <t>[3.49, 5.213]</t>
-  </si>
-  <si>
-    <t>2.6009995937347408</t>
-  </si>
-  <si>
-    <t>231.277</t>
-  </si>
-  <si>
-    <t>13483.0</t>
-  </si>
-  <si>
-    <t>275.0</t>
+    <t>c1cc(c(c(c1)Cl)NC(=O)c2ccncc2)Cl</t>
+  </si>
+  <si>
+    <t>3605943</t>
+  </si>
+  <si>
+    <t>COc1cccc(c1)Nc1ncnc2c1cccc2.Cl</t>
+  </si>
+  <si>
+    <t>[4.05]</t>
+  </si>
+  <si>
+    <t>3.138999938964844</t>
+  </si>
+  <si>
+    <t>287.744</t>
+  </si>
+  <si>
+    <t>119.7</t>
+  </si>
+  <si>
+    <t>16</t>
+  </si>
+  <si>
+    <t>COc1cccc(c1)Nc2c3ccccc3ncn2.Cl</t>
+  </si>
+  <si>
+    <t>1865544</t>
+  </si>
+  <si>
+    <t>OCCNc1ncnc2c1c(c1ccccc1)c(o2)c1ccccc1</t>
+  </si>
+  <si>
+    <t>[4.294]</t>
+  </si>
+  <si>
+    <t>3.0820000171661377</t>
+  </si>
+  <si>
+    <t>331.36800000000005</t>
+  </si>
+  <si>
+    <t>159.0</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>71</t>
+  </si>
+  <si>
+    <t>c1ccc(cc1)c2c3c(ncnc3oc2c4ccccc4)NCCO</t>
+  </si>
+  <si>
+    <t>1415762</t>
+  </si>
+  <si>
+    <t>c1ccc(cc1)CSc1nnc(o1)c1ccncc1</t>
+  </si>
+  <si>
+    <t>[4.902]</t>
+  </si>
+  <si>
+    <t>3.3059999942779537</t>
+  </si>
+  <si>
+    <t>269.322</t>
+  </si>
+  <si>
+    <t>170.0</t>
+  </si>
+  <si>
+    <t>30</t>
+  </si>
+  <si>
+    <t>17</t>
+  </si>
+  <si>
+    <t>c1ccc(cc1)CSc2nnc(o2)c3ccncc3</t>
+  </si>
+  <si>
+    <t>1444229</t>
+  </si>
+  <si>
+    <t>O=C(Nc1noc(c1)C(C)(C)C)Nc1ccc(cc1)F</t>
+  </si>
+  <si>
+    <t>[3.417]</t>
+  </si>
+  <si>
+    <t>3.4079995155334477</t>
+  </si>
+  <si>
+    <t>277.29400000000004</t>
+  </si>
+  <si>
+    <t>114.0</t>
+  </si>
+  <si>
+    <t>CC(C)(C)c1cc(no1)NC(=O)Nc2ccc(cc2)F</t>
+  </si>
+  <si>
+    <t>2546448</t>
+  </si>
+  <si>
+    <t>O=C(c1cccs1)Nc1nnc(s1)Cc1ccccc1</t>
+  </si>
+  <si>
+    <t>[7.12]</t>
+  </si>
+  <si>
+    <t>3.6050002574920654</t>
+  </si>
+  <si>
+    <t>301.387</t>
+  </si>
+  <si>
+    <t>379.0</t>
+  </si>
+  <si>
+    <t>18</t>
+  </si>
+  <si>
+    <t>c1ccc(cc1)Cc2nnc(s2)NC(=O)c3cccs3</t>
+  </si>
+  <si>
+    <t>1228629</t>
+  </si>
+  <si>
+    <t>Clc1ccc(cc1)CNc1ncnc2c1cccc2</t>
+  </si>
+  <si>
+    <t>[5.564]</t>
+  </si>
+  <si>
+    <t>3.523000240325928</t>
+  </si>
+  <si>
+    <t>269.72900000000004</t>
+  </si>
+  <si>
+    <t>415.5</t>
+  </si>
+  <si>
+    <t>c1ccc2c(c1)c(ncn2)NCc3ccc(cc3)Cl</t>
+  </si>
+  <si>
+    <t>30719859</t>
+  </si>
+  <si>
+    <t>Clc1ccc(o1)C(=O)Nc1ccccc1N1CCCCC1</t>
+  </si>
+  <si>
+    <t>[5.346]</t>
+  </si>
+  <si>
+    <t>3.794999837875366</t>
+  </si>
+  <si>
+    <t>304.771</t>
+  </si>
+  <si>
+    <t>424.3</t>
   </si>
   <si>
     <t>19</t>
   </si>
   <si>
-    <t>Cc1nnc2n1nc(s2)c3ccc(cc3)N</t>
-  </si>
-  <si>
-    <t>1503405</t>
-  </si>
-  <si>
-    <t>O=C(Nc1nc2c(s1)cccc2)CNC(=O)c1ccccc1</t>
-  </si>
-  <si>
-    <t>[8.672]</t>
-  </si>
-  <si>
-    <t>2.7179999351501465</t>
-  </si>
-  <si>
-    <t>311.358</t>
-  </si>
-  <si>
-    <t>149.1</t>
-  </si>
-  <si>
-    <t>6</t>
-  </si>
-  <si>
-    <t>14</t>
-  </si>
-  <si>
-    <t>c1ccc(cc1)C(=O)NCC(=O)Nc2nc3ccccc3s2</t>
-  </si>
-  <si>
-    <t>23354217</t>
-  </si>
-  <si>
-    <t>O=C(c1c(F)cccc1Cl)Nc1ccncc1</t>
-  </si>
-  <si>
-    <t>[4.714, 10.192]</t>
-  </si>
-  <si>
-    <t>2.7859997749328613</t>
-  </si>
-  <si>
-    <t>250.656</t>
-  </si>
-  <si>
-    <t>115.0</t>
-  </si>
-  <si>
-    <t>c1cc(c(c(c1)Cl)C(=O)Nc2ccncc2)F</t>
-  </si>
-  <si>
-    <t>17004732</t>
-  </si>
-  <si>
-    <t>Brc1cncc(c1)C(=O)Nc1cccc2c1nccc2</t>
-  </si>
-  <si>
-    <t>[4.001, 10.328]</t>
-  </si>
-  <si>
-    <t>2.922999620437622</t>
-  </si>
-  <si>
-    <t>328.163</t>
-  </si>
-  <si>
-    <t>406.0</t>
-  </si>
-  <si>
-    <t>37</t>
-  </si>
-  <si>
-    <t>15</t>
-  </si>
-  <si>
-    <t>c1cc2cccnc2c(c1)NC(=O)c3cc(cnc3)Br</t>
-  </si>
-  <si>
-    <t>18893169</t>
-  </si>
-  <si>
-    <t>O=C(c1cccc(c1Cl)Cl)Nc1ccncc1</t>
-  </si>
-  <si>
-    <t>[4.714, 10.167]</t>
-  </si>
-  <si>
-    <t>2.9270002841949463</t>
-  </si>
-  <si>
-    <t>267.111</t>
-  </si>
-  <si>
-    <t>104.0</t>
-  </si>
-  <si>
-    <t>c1cc(c(c(c1)Cl)Cl)C(=O)Nc2ccncc2</t>
-  </si>
-  <si>
-    <t>2266357</t>
-  </si>
-  <si>
-    <t>COc1cccc(c1)Nc1ncnc2c1cccc2.Cl</t>
-  </si>
-  <si>
-    <t>[4.05]</t>
-  </si>
-  <si>
-    <t>3.138999938964844</t>
-  </si>
-  <si>
-    <t>287.744</t>
-  </si>
-  <si>
-    <t>119.7</t>
-  </si>
-  <si>
-    <t>16</t>
-  </si>
-  <si>
-    <t>COc1cccc(c1)Nc2c3ccccc3ncn2.Cl</t>
-  </si>
-  <si>
-    <t>1865544</t>
-  </si>
-  <si>
-    <t>c1ccc(cc1)n1cnc2c1cccc2</t>
-  </si>
-  <si>
-    <t>[5.74]</t>
-  </si>
-  <si>
-    <t>3.1050000190734863</t>
-  </si>
-  <si>
-    <t>194.232</t>
-  </si>
-  <si>
-    <t>188.0</t>
-  </si>
-  <si>
-    <t>c1ccc(cc1)n2cnc3c2cccc3</t>
-  </si>
-  <si>
-    <t>1202048</t>
-  </si>
-  <si>
-    <t>c1ccc(cc1)CSc1nnc(o1)c1ccncc1</t>
-  </si>
-  <si>
-    <t>[4.902]</t>
-  </si>
-  <si>
-    <t>3.3059999942779537</t>
-  </si>
-  <si>
-    <t>269.322</t>
-  </si>
-  <si>
-    <t>170.0</t>
-  </si>
-  <si>
-    <t>30</t>
-  </si>
-  <si>
-    <t>17</t>
-  </si>
-  <si>
-    <t>c1ccc(cc1)CSc2nnc(o2)c3ccncc3</t>
-  </si>
-  <si>
-    <t>1444229</t>
-  </si>
-  <si>
-    <t>O=C(c1ccc(cc1)Oc1ccccc1)NCc1ccncc1</t>
-  </si>
-  <si>
-    <t>[5.124]</t>
-  </si>
-  <si>
-    <t>3.2410001754760738</t>
-  </si>
-  <si>
-    <t>304.343</t>
-  </si>
-  <si>
-    <t>211.0</t>
+    <t>c1ccc(c(c1)NC(=O)c2ccc(o2)Cl)N3CCCCC3</t>
+  </si>
+  <si>
+    <t>18908671</t>
+  </si>
+  <si>
+    <t>Cc1ccc(cc1)S(=O)(=O)Nc1cccc(c1)C(F)(F)F</t>
+  </si>
+  <si>
+    <t>[7.903]</t>
+  </si>
+  <si>
+    <t>3.747999668121338</t>
+  </si>
+  <si>
+    <t>315.311</t>
+  </si>
+  <si>
+    <t>527.0</t>
+  </si>
+  <si>
+    <t>24</t>
+  </si>
+  <si>
+    <t>Cc1ccc(cc1)S(=O)(=O)Nc2cccc(c2)C(F)(F)F</t>
+  </si>
+  <si>
+    <t>1377874</t>
+  </si>
+  <si>
+    <t>O=C1S/C(=C/c2ccc(o2)c2ccc(c(c2)Cl)F)/C(=O)N1</t>
+  </si>
+  <si>
+    <t>[8.052]</t>
+  </si>
+  <si>
+    <t>3.9079997539520255</t>
+  </si>
+  <si>
+    <t>323.7270000000001</t>
+  </si>
+  <si>
+    <t>125.0</t>
+  </si>
+  <si>
+    <t>c1cc(c(cc1c2ccc(o2)/C=C/3\C(=O)NC(=O)S3)Cl)F</t>
+  </si>
+  <si>
+    <t>25775231</t>
+  </si>
+  <si>
+    <t>Brc1ccc(o1)C(=O)Nc1ccccc1N1CCCCC1</t>
+  </si>
+  <si>
+    <t>3.9770002365112314</t>
+  </si>
+  <si>
+    <t>349.222</t>
+  </si>
+  <si>
+    <t>530.0</t>
+  </si>
+  <si>
+    <t>c1ccc(c(c1)NC(=O)c2ccc(o2)Br)N3CCCCC3</t>
+  </si>
+  <si>
+    <t>1716329</t>
+  </si>
+  <si>
+    <t>FC(c1ccc(cc1)c1nnc2n1nc(cc2)NC1CC1)(F)F</t>
+  </si>
+  <si>
+    <t>[4.394]</t>
+  </si>
+  <si>
+    <t>4.128999710083009</t>
+  </si>
+  <si>
+    <t>319.284</t>
+  </si>
+  <si>
+    <t>3175.0</t>
   </si>
   <si>
     <t>32</t>
-  </si>
-  <si>
-    <t>c1ccc(cc1)Oc2ccc(cc2)C(=O)NCc3ccncc3</t>
-  </si>
-  <si>
-    <t>3374919</t>
-  </si>
-  <si>
-    <t>O=C(c1cccs1)Nc1nnc(s1)Cc1ccccc1</t>
-  </si>
-  <si>
-    <t>[7.12]</t>
-  </si>
-  <si>
-    <t>3.6050002574920654</t>
-  </si>
-  <si>
-    <t>301.387</t>
-  </si>
-  <si>
-    <t>379.0</t>
-  </si>
-  <si>
-    <t>5</t>
-  </si>
-  <si>
-    <t>18</t>
-  </si>
-  <si>
-    <t>c1ccc(cc1)Cc2nnc(s2)NC(=O)c3cccs3</t>
-  </si>
-  <si>
-    <t>1228629</t>
-  </si>
-  <si>
-    <t>Clc1ccc(cc1)CNc1ncnc2c1cccc2</t>
-  </si>
-  <si>
-    <t>[5.564]</t>
-  </si>
-  <si>
-    <t>3.523000240325928</t>
-  </si>
-  <si>
-    <t>269.72900000000004</t>
-  </si>
-  <si>
-    <t>415.5</t>
-  </si>
-  <si>
-    <t>c1ccc2c(c1)c(ncn2)NCc3ccc(cc3)Cl</t>
-  </si>
-  <si>
-    <t>30719859</t>
-  </si>
-  <si>
-    <t>Clc1ccc(o1)C(=O)Nc1ccccc1N1CCCCC1</t>
-  </si>
-  <si>
-    <t>[5.346]</t>
-  </si>
-  <si>
-    <t>3.794999837875366</t>
-  </si>
-  <si>
-    <t>304.771</t>
-  </si>
-  <si>
-    <t>424.3</t>
-  </si>
-  <si>
-    <t>c1ccc(c(c1)NC(=O)c2ccc(o2)Cl)N3CCCCC3</t>
-  </si>
-  <si>
-    <t>18908671</t>
-  </si>
-  <si>
-    <t>Cc1ccc(cc1)S(=O)(=O)Nc1cccc(c1)C(F)(F)F</t>
-  </si>
-  <si>
-    <t>[7.903]</t>
-  </si>
-  <si>
-    <t>3.747999668121338</t>
-  </si>
-  <si>
-    <t>315.311</t>
-  </si>
-  <si>
-    <t>527.0</t>
-  </si>
-  <si>
-    <t>24</t>
-  </si>
-  <si>
-    <t>Cc1ccc(cc1)S(=O)(=O)Nc2cccc(c2)C(F)(F)F</t>
-  </si>
-  <si>
-    <t>1377874</t>
-  </si>
-  <si>
-    <t>O=C1S/C(=C/c2ccc(o2)c2ccc(c(c2)Cl)F)/C(=O)N1</t>
-  </si>
-  <si>
-    <t>[8.052]</t>
-  </si>
-  <si>
-    <t>3.9079997539520255</t>
-  </si>
-  <si>
-    <t>323.7270000000001</t>
-  </si>
-  <si>
-    <t>125.0</t>
-  </si>
-  <si>
-    <t>c1cc(c(cc1c2ccc(o2)/C=C/3\C(=O)NC(=O)S3)Cl)F</t>
-  </si>
-  <si>
-    <t>25775231</t>
-  </si>
-  <si>
-    <t>FC(c1ccc(cc1)c1nnc2n1nc(cc2)NC1CC1)(F)F</t>
-  </si>
-  <si>
-    <t>[4.394]</t>
-  </si>
-  <si>
-    <t>4.128999710083009</t>
-  </si>
-  <si>
-    <t>319.284</t>
-  </si>
-  <si>
-    <t>3175.0</t>
   </si>
   <si>
     <t>21</t>
@@ -2252,16 +2243,16 @@
         <v>23</v>
       </c>
       <c r="I5" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="J5" s="2" t="s">
         <v>48</v>
-      </c>
-      <c r="J5" s="2" t="s">
-        <v>49</v>
       </c>
       <c r="K5" s="2" t="s">
         <v>26</v>
       </c>
       <c r="L5" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="M5" s="2" t="s">
         <v>28</v>
@@ -2270,121 +2261,121 @@
         <v>29</v>
       </c>
       <c r="O5" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="P5" s="2" t="s">
         <v>51</v>
-      </c>
-      <c r="P5" s="2" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="6" spans="1:16" s="3" customFormat="1" ht="187.5" customHeight="1">
       <c r="B6" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="C6" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="D6" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="E6" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="E6" s="3" t="s">
+      <c r="F6" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="F6" s="3" t="s">
+      <c r="G6" s="3" t="s">
         <v>57</v>
-      </c>
-      <c r="G6" s="3" t="s">
-        <v>58</v>
       </c>
       <c r="H6" s="3" t="s">
         <v>23</v>
       </c>
       <c r="I6" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="J6" s="3" t="s">
         <v>59</v>
-      </c>
-      <c r="J6" s="3" t="s">
-        <v>60</v>
       </c>
       <c r="K6" s="3" t="s">
         <v>26</v>
       </c>
       <c r="L6" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="M6" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="N6" s="3" t="s">
         <v>29</v>
       </c>
       <c r="O6" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="P6" s="3" t="s">
         <v>61</v>
-      </c>
-      <c r="P6" s="3" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="7" spans="1:16" s="2" customFormat="1" ht="187.5" customHeight="1">
       <c r="B7" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="C7" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="D7" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="D7" s="2" t="s">
+      <c r="E7" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="E7" s="2" t="s">
+      <c r="F7" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="F7" s="2" t="s">
+      <c r="G7" s="2" t="s">
         <v>67</v>
-      </c>
-      <c r="G7" s="2" t="s">
-        <v>68</v>
       </c>
       <c r="H7" s="2" t="s">
         <v>23</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>28</v>
+        <v>58</v>
       </c>
       <c r="J7" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="K7" s="2" t="s">
         <v>26</v>
       </c>
       <c r="L7" s="2" t="s">
-        <v>70</v>
+        <v>49</v>
       </c>
       <c r="M7" s="2" t="s">
-        <v>28</v>
+        <v>69</v>
       </c>
       <c r="N7" s="2" t="s">
         <v>29</v>
       </c>
       <c r="O7" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="P7" s="2" t="s">
         <v>71</v>
-      </c>
-      <c r="P7" s="2" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="8" spans="1:16" s="3" customFormat="1" ht="187.5" customHeight="1">
       <c r="B8" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="C8" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="D8" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="D8" s="3" t="s">
+      <c r="E8" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="E8" s="3" t="s">
+      <c r="F8" s="3" t="s">
         <v>76</v>
-      </c>
-      <c r="F8" s="3" t="s">
-        <v>77</v>
       </c>
       <c r="G8" s="3" t="s">
         <v>47</v>
@@ -2393,280 +2384,280 @@
         <v>23</v>
       </c>
       <c r="I8" s="3" t="s">
-        <v>59</v>
+        <v>28</v>
       </c>
       <c r="J8" s="3" t="s">
-        <v>78</v>
+        <v>48</v>
       </c>
       <c r="K8" s="3" t="s">
         <v>26</v>
       </c>
       <c r="L8" s="3" t="s">
-        <v>70</v>
+        <v>77</v>
       </c>
       <c r="M8" s="3" t="s">
-        <v>59</v>
+        <v>28</v>
       </c>
       <c r="N8" s="3" t="s">
         <v>29</v>
       </c>
       <c r="O8" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="P8" s="3" t="s">
         <v>79</v>
-      </c>
-      <c r="P8" s="3" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="9" spans="1:16" s="2" customFormat="1" ht="187.5" customHeight="1">
       <c r="B9" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="D9" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="E9" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="D9" s="2" t="s">
+      <c r="F9" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="E9" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="F9" s="2" t="s">
-        <v>85</v>
-      </c>
       <c r="G9" s="2" t="s">
-        <v>68</v>
+        <v>57</v>
       </c>
       <c r="H9" s="2" t="s">
         <v>23</v>
       </c>
       <c r="I9" s="2" t="s">
-        <v>28</v>
+        <v>69</v>
       </c>
       <c r="J9" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="K9" s="2" t="s">
         <v>26</v>
       </c>
       <c r="L9" s="2" t="s">
-        <v>60</v>
+        <v>77</v>
       </c>
       <c r="M9" s="2" t="s">
-        <v>28</v>
+        <v>58</v>
       </c>
       <c r="N9" s="2" t="s">
         <v>29</v>
       </c>
       <c r="O9" s="2" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="P9" s="2" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="10" spans="1:16" s="3" customFormat="1" ht="187.5" customHeight="1">
       <c r="B10" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="D10" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="C10" s="3" t="s">
+      <c r="E10" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="F10" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="D10" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="E10" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="F10" s="3" t="s">
-        <v>92</v>
-      </c>
       <c r="G10" s="3" t="s">
-        <v>47</v>
+        <v>67</v>
       </c>
       <c r="H10" s="3" t="s">
         <v>23</v>
       </c>
       <c r="I10" s="3" t="s">
-        <v>48</v>
+        <v>69</v>
       </c>
       <c r="J10" s="3" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="K10" s="3" t="s">
         <v>26</v>
       </c>
       <c r="L10" s="3" t="s">
-        <v>60</v>
+        <v>91</v>
       </c>
       <c r="M10" s="3" t="s">
-        <v>59</v>
+        <v>28</v>
       </c>
       <c r="N10" s="3" t="s">
         <v>29</v>
       </c>
       <c r="O10" s="3" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="P10" s="3" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="11" spans="1:16" s="2" customFormat="1" ht="187.5" customHeight="1">
       <c r="B11" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="D11" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="C11" s="2" t="s">
+      <c r="E11" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="D11" s="2" t="s">
+      <c r="F11" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="E11" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="F11" s="2" t="s">
-        <v>99</v>
-      </c>
       <c r="G11" s="2" t="s">
-        <v>100</v>
+        <v>37</v>
       </c>
       <c r="H11" s="2" t="s">
         <v>23</v>
       </c>
       <c r="I11" s="2" t="s">
-        <v>48</v>
+        <v>27</v>
       </c>
       <c r="J11" s="2" t="s">
-        <v>101</v>
+        <v>90</v>
       </c>
       <c r="K11" s="2" t="s">
         <v>26</v>
       </c>
       <c r="L11" s="2" t="s">
-        <v>102</v>
+        <v>91</v>
       </c>
       <c r="M11" s="2" t="s">
-        <v>28</v>
+        <v>58</v>
       </c>
       <c r="N11" s="2" t="s">
         <v>29</v>
       </c>
       <c r="O11" s="2" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="P11" s="2" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
     </row>
     <row r="12" spans="1:16" s="3" customFormat="1" ht="187.5" customHeight="1">
       <c r="B12" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="F12" s="3" t="s">
         <v>105</v>
       </c>
-      <c r="C12" s="3" t="s">
-        <v>106</v>
-      </c>
-      <c r="D12" s="3" t="s">
-        <v>107</v>
-      </c>
-      <c r="E12" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="F12" s="3" t="s">
-        <v>109</v>
-      </c>
       <c r="G12" s="3" t="s">
-        <v>110</v>
+        <v>47</v>
       </c>
       <c r="H12" s="3" t="s">
         <v>23</v>
       </c>
       <c r="I12" s="3" t="s">
-        <v>28</v>
+        <v>106</v>
       </c>
       <c r="J12" s="3" t="s">
-        <v>111</v>
+        <v>68</v>
       </c>
       <c r="K12" s="3" t="s">
         <v>26</v>
       </c>
       <c r="L12" s="3" t="s">
-        <v>102</v>
+        <v>107</v>
       </c>
       <c r="M12" s="3" t="s">
-        <v>59</v>
+        <v>28</v>
       </c>
       <c r="N12" s="3" t="s">
         <v>29</v>
       </c>
       <c r="O12" s="3" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="P12" s="3" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
     </row>
     <row r="13" spans="1:16" s="2" customFormat="1" ht="187.5" customHeight="1">
       <c r="B13" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="F13" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="C13" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="F13" s="2" t="s">
-        <v>118</v>
-      </c>
       <c r="G13" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="H13" s="2" t="s">
         <v>23</v>
       </c>
       <c r="I13" s="2" t="s">
-        <v>119</v>
+        <v>69</v>
       </c>
       <c r="J13" s="2" t="s">
-        <v>93</v>
+        <v>115</v>
       </c>
       <c r="K13" s="2" t="s">
         <v>26</v>
       </c>
       <c r="L13" s="2" t="s">
-        <v>120</v>
+        <v>107</v>
       </c>
       <c r="M13" s="2" t="s">
-        <v>28</v>
+        <v>58</v>
       </c>
       <c r="N13" s="2" t="s">
         <v>29</v>
       </c>
       <c r="O13" s="2" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="P13" s="2" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
     </row>
     <row r="14" spans="1:16" s="3" customFormat="1" ht="187.5" customHeight="1">
       <c r="B14" s="3" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="G14" s="3" t="s">
         <v>47</v>
@@ -2675,92 +2666,92 @@
         <v>23</v>
       </c>
       <c r="I14" s="3" t="s">
-        <v>48</v>
+        <v>69</v>
       </c>
       <c r="J14" s="3" t="s">
-        <v>49</v>
+        <v>123</v>
       </c>
       <c r="K14" s="3" t="s">
         <v>26</v>
       </c>
       <c r="L14" s="3" t="s">
-        <v>120</v>
+        <v>124</v>
       </c>
       <c r="M14" s="3" t="s">
-        <v>59</v>
+        <v>28</v>
       </c>
       <c r="N14" s="3" t="s">
         <v>29</v>
       </c>
       <c r="O14" s="3" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="P14" s="3" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
     </row>
     <row r="15" spans="1:16" s="2" customFormat="1" ht="187.5" customHeight="1">
       <c r="B15" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="E15" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="C15" s="2" t="s">
+      <c r="F15" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="D15" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="E15" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="F15" s="2" t="s">
-        <v>134</v>
-      </c>
       <c r="G15" s="2" t="s">
-        <v>68</v>
+        <v>57</v>
       </c>
       <c r="H15" s="2" t="s">
         <v>23</v>
       </c>
       <c r="I15" s="2" t="s">
-        <v>48</v>
+        <v>69</v>
       </c>
       <c r="J15" s="2" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="K15" s="2" t="s">
         <v>26</v>
       </c>
       <c r="L15" s="2" t="s">
-        <v>136</v>
+        <v>124</v>
       </c>
       <c r="M15" s="2" t="s">
-        <v>28</v>
+        <v>58</v>
       </c>
       <c r="N15" s="2" t="s">
         <v>29</v>
       </c>
       <c r="O15" s="2" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="P15" s="2" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
     </row>
     <row r="16" spans="1:16" s="3" customFormat="1" ht="187.5" customHeight="1">
       <c r="B16" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="F16" s="3" t="s">
         <v>139</v>
-      </c>
-      <c r="C16" s="3" t="s">
-        <v>140</v>
-      </c>
-      <c r="D16" s="3" t="s">
-        <v>141</v>
-      </c>
-      <c r="E16" s="3" t="s">
-        <v>142</v>
-      </c>
-      <c r="F16" s="3" t="s">
-        <v>143</v>
       </c>
       <c r="G16" s="3" t="s">
         <v>47</v>
@@ -2769,113 +2760,113 @@
         <v>23</v>
       </c>
       <c r="I16" s="3" t="s">
-        <v>48</v>
+        <v>69</v>
       </c>
       <c r="J16" s="3" t="s">
-        <v>49</v>
+        <v>90</v>
       </c>
       <c r="K16" s="3" t="s">
         <v>26</v>
       </c>
       <c r="L16" s="3" t="s">
-        <v>136</v>
+        <v>140</v>
       </c>
       <c r="M16" s="3" t="s">
-        <v>59</v>
+        <v>28</v>
       </c>
       <c r="N16" s="3" t="s">
         <v>29</v>
       </c>
       <c r="O16" s="3" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="P16" s="3" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
     </row>
     <row r="17" spans="2:16" s="2" customFormat="1" ht="187.5" customHeight="1">
       <c r="B17" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="E17" s="2" t="s">
         <v>146</v>
       </c>
-      <c r="C17" s="2" t="s">
+      <c r="F17" s="2" t="s">
         <v>147</v>
       </c>
-      <c r="D17" s="2" t="s">
-        <v>148</v>
-      </c>
-      <c r="E17" s="2" t="s">
-        <v>149</v>
-      </c>
-      <c r="F17" s="2" t="s">
-        <v>150</v>
-      </c>
       <c r="G17" s="2" t="s">
-        <v>68</v>
+        <v>57</v>
       </c>
       <c r="H17" s="2" t="s">
         <v>23</v>
       </c>
       <c r="I17" s="2" t="s">
-        <v>48</v>
+        <v>148</v>
       </c>
       <c r="J17" s="2" t="s">
-        <v>101</v>
+        <v>149</v>
       </c>
       <c r="K17" s="2" t="s">
         <v>26</v>
       </c>
       <c r="L17" s="2" t="s">
-        <v>151</v>
+        <v>140</v>
       </c>
       <c r="M17" s="2" t="s">
-        <v>28</v>
+        <v>58</v>
       </c>
       <c r="N17" s="2" t="s">
         <v>29</v>
       </c>
       <c r="O17" s="2" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="P17" s="2" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="18" spans="2:16" s="3" customFormat="1" ht="187.5" customHeight="1">
       <c r="B18" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="D18" s="3" t="s">
         <v>154</v>
       </c>
-      <c r="C18" s="3" t="s">
+      <c r="E18" s="3" t="s">
         <v>155</v>
       </c>
-      <c r="D18" s="3" t="s">
+      <c r="F18" s="3" t="s">
         <v>156</v>
       </c>
-      <c r="E18" s="3" t="s">
-        <v>157</v>
-      </c>
-      <c r="F18" s="3" t="s">
-        <v>158</v>
-      </c>
       <c r="G18" s="3" t="s">
-        <v>47</v>
+        <v>57</v>
       </c>
       <c r="H18" s="3" t="s">
         <v>23</v>
       </c>
       <c r="I18" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="J18" s="3" t="s">
-        <v>69</v>
+        <v>157</v>
       </c>
       <c r="K18" s="3" t="s">
         <v>26</v>
       </c>
       <c r="L18" s="3" t="s">
-        <v>151</v>
+        <v>158</v>
       </c>
       <c r="M18" s="3" t="s">
-        <v>59</v>
+        <v>28</v>
       </c>
       <c r="N18" s="3" t="s">
         <v>29</v>
@@ -2904,51 +2895,51 @@
         <v>165</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>47</v>
+        <v>57</v>
       </c>
       <c r="H19" s="2" t="s">
         <v>23</v>
       </c>
       <c r="I19" s="2" t="s">
-        <v>27</v>
+        <v>148</v>
       </c>
       <c r="J19" s="2" t="s">
-        <v>166</v>
+        <v>140</v>
       </c>
       <c r="K19" s="2" t="s">
         <v>26</v>
       </c>
       <c r="L19" s="2" t="s">
-        <v>167</v>
+        <v>158</v>
       </c>
       <c r="M19" s="2" t="s">
-        <v>28</v>
+        <v>58</v>
       </c>
       <c r="N19" s="2" t="s">
         <v>29</v>
       </c>
       <c r="O19" s="2" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="P19" s="2" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
     </row>
     <row r="20" spans="2:16" s="3" customFormat="1" ht="187.5" customHeight="1">
       <c r="B20" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>169</v>
+      </c>
+      <c r="D20" s="3" t="s">
         <v>170</v>
       </c>
-      <c r="C20" s="3" t="s">
+      <c r="E20" s="3" t="s">
         <v>171</v>
       </c>
-      <c r="D20" s="3" t="s">
+      <c r="F20" s="3" t="s">
         <v>172</v>
-      </c>
-      <c r="E20" s="3" t="s">
-        <v>173</v>
-      </c>
-      <c r="F20" s="3" t="s">
-        <v>174</v>
       </c>
       <c r="G20" s="3" t="s">
         <v>47</v>
@@ -2957,142 +2948,142 @@
         <v>23</v>
       </c>
       <c r="I20" s="3" t="s">
-        <v>119</v>
+        <v>148</v>
       </c>
       <c r="J20" s="3" t="s">
-        <v>175</v>
+        <v>107</v>
       </c>
       <c r="K20" s="3" t="s">
         <v>26</v>
       </c>
       <c r="L20" s="3" t="s">
-        <v>167</v>
+        <v>173</v>
       </c>
       <c r="M20" s="3" t="s">
-        <v>59</v>
+        <v>28</v>
       </c>
       <c r="N20" s="3" t="s">
         <v>29</v>
       </c>
       <c r="O20" s="3" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="P20" s="3" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
     </row>
     <row r="21" spans="2:16" s="2" customFormat="1" ht="187.5" customHeight="1">
       <c r="B21" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="D21" s="2" t="s">
         <v>178</v>
       </c>
-      <c r="C21" s="2" t="s">
+      <c r="E21" s="2" t="s">
         <v>179</v>
       </c>
-      <c r="D21" s="2" t="s">
+      <c r="F21" s="2" t="s">
         <v>180</v>
       </c>
-      <c r="E21" s="2" t="s">
-        <v>181</v>
-      </c>
-      <c r="F21" s="2" t="s">
-        <v>182</v>
-      </c>
       <c r="G21" s="2" t="s">
-        <v>68</v>
+        <v>47</v>
       </c>
       <c r="H21" s="2" t="s">
         <v>23</v>
       </c>
       <c r="I21" s="2" t="s">
-        <v>183</v>
+        <v>69</v>
       </c>
       <c r="J21" s="2" t="s">
-        <v>120</v>
+        <v>90</v>
       </c>
       <c r="K21" s="2" t="s">
         <v>26</v>
       </c>
       <c r="L21" s="2" t="s">
-        <v>184</v>
+        <v>173</v>
       </c>
       <c r="M21" s="2" t="s">
-        <v>28</v>
+        <v>58</v>
       </c>
       <c r="N21" s="2" t="s">
         <v>29</v>
       </c>
       <c r="O21" s="2" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="P21" s="2" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
     </row>
     <row r="22" spans="2:16" s="3" customFormat="1" ht="187.5" customHeight="1">
       <c r="B22" s="3" t="s">
+        <v>183</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>185</v>
+      </c>
+      <c r="E22" s="3" t="s">
+        <v>186</v>
+      </c>
+      <c r="F22" s="3" t="s">
         <v>187</v>
       </c>
-      <c r="C22" s="3" t="s">
-        <v>188</v>
-      </c>
-      <c r="D22" s="3" t="s">
-        <v>189</v>
-      </c>
-      <c r="E22" s="3" t="s">
-        <v>190</v>
-      </c>
-      <c r="F22" s="3" t="s">
-        <v>191</v>
-      </c>
       <c r="G22" s="3" t="s">
-        <v>68</v>
+        <v>47</v>
       </c>
       <c r="H22" s="3" t="s">
         <v>23</v>
       </c>
       <c r="I22" s="3" t="s">
-        <v>48</v>
+        <v>27</v>
       </c>
       <c r="J22" s="3" t="s">
-        <v>101</v>
+        <v>173</v>
       </c>
       <c r="K22" s="3" t="s">
         <v>26</v>
       </c>
       <c r="L22" s="3" t="s">
-        <v>184</v>
+        <v>188</v>
       </c>
       <c r="M22" s="3" t="s">
-        <v>59</v>
+        <v>28</v>
       </c>
       <c r="N22" s="3" t="s">
         <v>29</v>
       </c>
       <c r="O22" s="3" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="P22" s="3" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
     </row>
     <row r="23" spans="2:16" s="2" customFormat="1" ht="187.5" customHeight="1">
       <c r="B23" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="E23" s="2" t="s">
         <v>194</v>
       </c>
-      <c r="C23" s="2" t="s">
+      <c r="F23" s="2" t="s">
         <v>195</v>
       </c>
-      <c r="D23" s="2" t="s">
-        <v>196</v>
-      </c>
-      <c r="E23" s="2" t="s">
-        <v>197</v>
-      </c>
-      <c r="F23" s="2" t="s">
-        <v>198</v>
-      </c>
       <c r="G23" s="2" t="s">
-        <v>68</v>
+        <v>57</v>
       </c>
       <c r="H23" s="2" t="s">
         <v>23</v>
@@ -3101,136 +3092,136 @@
         <v>27</v>
       </c>
       <c r="J23" s="2" t="s">
-        <v>184</v>
+        <v>196</v>
       </c>
       <c r="K23" s="2" t="s">
         <v>26</v>
       </c>
       <c r="L23" s="2" t="s">
-        <v>111</v>
+        <v>188</v>
       </c>
       <c r="M23" s="2" t="s">
-        <v>28</v>
+        <v>58</v>
       </c>
       <c r="N23" s="2" t="s">
         <v>29</v>
       </c>
       <c r="O23" s="2" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="P23" s="2" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
     </row>
     <row r="24" spans="2:16" s="3" customFormat="1" ht="187.5" customHeight="1">
       <c r="B24" s="3" t="s">
+        <v>199</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>200</v>
+      </c>
+      <c r="D24" s="3" t="s">
         <v>201</v>
       </c>
-      <c r="C24" s="3" t="s">
+      <c r="E24" s="3" t="s">
         <v>202</v>
       </c>
-      <c r="D24" s="3" t="s">
+      <c r="F24" s="3" t="s">
         <v>203</v>
       </c>
-      <c r="E24" s="3" t="s">
-        <v>204</v>
-      </c>
-      <c r="F24" s="3" t="s">
-        <v>205</v>
-      </c>
       <c r="G24" s="3" t="s">
-        <v>47</v>
+        <v>57</v>
       </c>
       <c r="H24" s="3" t="s">
         <v>23</v>
       </c>
       <c r="I24" s="3" t="s">
-        <v>27</v>
+        <v>58</v>
       </c>
       <c r="J24" s="3" t="s">
-        <v>206</v>
+        <v>38</v>
       </c>
       <c r="K24" s="3" t="s">
         <v>26</v>
       </c>
       <c r="L24" s="3" t="s">
-        <v>111</v>
+        <v>132</v>
       </c>
       <c r="M24" s="3" t="s">
-        <v>59</v>
+        <v>28</v>
       </c>
       <c r="N24" s="3" t="s">
         <v>29</v>
       </c>
       <c r="O24" s="3" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="P24" s="3" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
     </row>
     <row r="25" spans="2:16" s="2" customFormat="1" ht="187.5" customHeight="1">
       <c r="B25" s="2" t="s">
+        <v>206</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>207</v>
+      </c>
+      <c r="E25" s="2" t="s">
+        <v>208</v>
+      </c>
+      <c r="F25" s="2" t="s">
         <v>209</v>
       </c>
-      <c r="C25" s="2" t="s">
-        <v>210</v>
-      </c>
-      <c r="D25" s="2" t="s">
-        <v>211</v>
-      </c>
-      <c r="E25" s="2" t="s">
-        <v>212</v>
-      </c>
-      <c r="F25" s="2" t="s">
-        <v>213</v>
-      </c>
       <c r="G25" s="2" t="s">
-        <v>47</v>
+        <v>57</v>
       </c>
       <c r="H25" s="2" t="s">
         <v>23</v>
       </c>
       <c r="I25" s="2" t="s">
-        <v>59</v>
+        <v>27</v>
       </c>
       <c r="J25" s="2" t="s">
-        <v>38</v>
+        <v>173</v>
       </c>
       <c r="K25" s="2" t="s">
         <v>26</v>
       </c>
       <c r="L25" s="2" t="s">
-        <v>49</v>
+        <v>132</v>
       </c>
       <c r="M25" s="2" t="s">
-        <v>28</v>
+        <v>58</v>
       </c>
       <c r="N25" s="2" t="s">
         <v>29</v>
       </c>
       <c r="O25" s="2" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="P25" s="2" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
     </row>
     <row r="26" spans="2:16" s="3" customFormat="1" ht="187.5" customHeight="1">
       <c r="B26" s="3" t="s">
+        <v>212</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>213</v>
+      </c>
+      <c r="D26" s="3" t="s">
+        <v>214</v>
+      </c>
+      <c r="E26" s="3" t="s">
+        <v>215</v>
+      </c>
+      <c r="F26" s="3" t="s">
         <v>216</v>
-      </c>
-      <c r="C26" s="3" t="s">
-        <v>217</v>
-      </c>
-      <c r="D26" s="3" t="s">
-        <v>218</v>
-      </c>
-      <c r="E26" s="3" t="s">
-        <v>219</v>
-      </c>
-      <c r="F26" s="3" t="s">
-        <v>220</v>
       </c>
       <c r="G26" s="3" t="s">
         <v>37</v>
@@ -3242,13 +3233,13 @@
         <v>27</v>
       </c>
       <c r="J26" s="3" t="s">
-        <v>175</v>
+        <v>217</v>
       </c>
       <c r="K26" s="3" t="s">
         <v>26</v>
       </c>
       <c r="L26" s="3" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="M26" s="3" t="s">
         <v>28</v>
@@ -3257,45 +3248,45 @@
         <v>29</v>
       </c>
       <c r="O26" s="3" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="P26" s="3" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
     </row>
     <row r="27" spans="2:16" s="2" customFormat="1" ht="187.5" customHeight="1">
       <c r="B27" s="2" t="s">
+        <v>221</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>223</v>
+      </c>
+      <c r="E27" s="2" t="s">
         <v>224</v>
       </c>
-      <c r="C27" s="2" t="s">
+      <c r="F27" s="2" t="s">
         <v>225</v>
       </c>
-      <c r="D27" s="2" t="s">
+      <c r="G27" s="2" t="s">
         <v>226</v>
-      </c>
-      <c r="E27" s="2" t="s">
-        <v>227</v>
-      </c>
-      <c r="F27" s="2" t="s">
-        <v>228</v>
-      </c>
-      <c r="G27" s="2" t="s">
-        <v>229</v>
       </c>
       <c r="H27" s="2" t="s">
         <v>23</v>
       </c>
       <c r="I27" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="J27" s="2" t="s">
-        <v>206</v>
+        <v>196</v>
       </c>
       <c r="K27" s="2" t="s">
         <v>26</v>
       </c>
       <c r="L27" s="2" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="M27" s="2" t="s">
         <v>28</v>
@@ -3304,10 +3295,10 @@
         <v>29</v>
       </c>
       <c r="O27" s="2" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="P27" s="2" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Round3: Filter compounds with Chemspider logPs.
</commit_message>
<xml_diff>
--- a/compound_selection/zinc15_eMolecules_intersection_set/20170807_zinc15_eMolecules_subset_depiction/df_frag_final_oe.xlsx
+++ b/compound_selection/zinc15_eMolecules_intersection_set/20170807_zinc15_eMolecules_subset_depiction/df_frag_final_oe.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="392" uniqueCount="230">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="392" uniqueCount="231">
   <si>
     <t>df_frag_final_oe.csv</t>
   </si>
@@ -202,90 +202,72 @@
     <t>37053191</t>
   </si>
   <si>
-    <t>CCn1c(nc2c1cccc2)c1nonc1N</t>
+    <t>Nc1ccc2c(c1)ncn2c1ccccc1</t>
+  </si>
+  <si>
+    <t>[6.348]</t>
+  </si>
+  <si>
+    <t>2.3329999446868896</t>
+  </si>
+  <si>
+    <t>209.247</t>
+  </si>
+  <si>
+    <t>50213.0</t>
+  </si>
+  <si>
+    <t>12</t>
+  </si>
+  <si>
+    <t>c1ccc(cc1)n2cnc3c2ccc(c3)N</t>
+  </si>
+  <si>
+    <t>31653344</t>
+  </si>
+  <si>
+    <t>Nc1nonc1c1nc2c(n1CC1CC1)cccc2</t>
   </si>
   <si>
     <t>[4.082]</t>
   </si>
   <si>
-    <t>2.068000078201294</t>
-  </si>
-  <si>
-    <t>229.238</t>
-  </si>
-  <si>
-    <t>385.3</t>
+    <t>2.43999981880188</t>
+  </si>
+  <si>
+    <t>255.275</t>
+  </si>
+  <si>
+    <t>300.0</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>28</t>
+  </si>
+  <si>
+    <t>c1ccc2c(c1)nc(n2CC3CC3)c4c(non4)N</t>
+  </si>
+  <si>
+    <t>8332960</t>
+  </si>
+  <si>
+    <t>O=C(c1n[nH]c2c1cccc2)Nc1ccccc1</t>
+  </si>
+  <si>
+    <t>[8.398]</t>
+  </si>
+  <si>
+    <t>2.6429998874664307</t>
+  </si>
+  <si>
+    <t>762.8</t>
   </si>
   <si>
     <t>223.0</t>
   </si>
   <si>
-    <t>28</t>
-  </si>
-  <si>
-    <t>3</t>
-  </si>
-  <si>
-    <t>CCn1c2ccccc2nc1c3c(non3)N</t>
-  </si>
-  <si>
-    <t>1360661</t>
-  </si>
-  <si>
-    <t>Nc1ccc2c(c1)ncn2c1ccccc1</t>
-  </si>
-  <si>
-    <t>[6.348]</t>
-  </si>
-  <si>
-    <t>2.3329999446868896</t>
-  </si>
-  <si>
-    <t>209.247</t>
-  </si>
-  <si>
-    <t>50213.0</t>
-  </si>
-  <si>
-    <t>12</t>
-  </si>
-  <si>
-    <t>c1ccc(cc1)n2cnc3c2ccc(c3)N</t>
-  </si>
-  <si>
-    <t>31653344</t>
-  </si>
-  <si>
-    <t>Nc1nonc1c1nc2c(n1CC1CC1)cccc2</t>
-  </si>
-  <si>
-    <t>2.43999981880188</t>
-  </si>
-  <si>
-    <t>255.275</t>
-  </si>
-  <si>
-    <t>300.0</t>
-  </si>
-  <si>
-    <t>c1ccc2c(c1)nc(n2CC3CC3)c4c(non4)N</t>
-  </si>
-  <si>
-    <t>8332960</t>
-  </si>
-  <si>
-    <t>O=C(c1n[nH]c2c1cccc2)Nc1ccccc1</t>
-  </si>
-  <si>
-    <t>[8.398]</t>
-  </si>
-  <si>
-    <t>2.6429998874664307</t>
-  </si>
-  <si>
-    <t>762.8</t>
-  </si>
-  <si>
     <t>36</t>
   </si>
   <si>
@@ -397,259 +379,283 @@
     <t>18893169</t>
   </si>
   <si>
-    <t>O=C(c1ccncc1)Nc1c(Cl)cccc1Cl</t>
-  </si>
-  <si>
-    <t>[3.163, 9.847]</t>
-  </si>
-  <si>
-    <t>2.9270000457763667</t>
-  </si>
-  <si>
-    <t>267.111</t>
-  </si>
-  <si>
-    <t>109.0</t>
+    <t>Nc1cc(C)c(c(c1)c1oc2c(n1)ccc(c2)C)O</t>
+  </si>
+  <si>
+    <t>[5.184, 8.99]</t>
+  </si>
+  <si>
+    <t>2.880000114440918</t>
+  </si>
+  <si>
+    <t>254.284</t>
+  </si>
+  <si>
+    <t>3132.0</t>
+  </si>
+  <si>
+    <t>Cc1ccc2c(c1)oc(n2)c3cc(cc(c3O)C)N</t>
+  </si>
+  <si>
+    <t>1532460</t>
+  </si>
+  <si>
+    <t>COc1cccc(c1)Nc1ncnc2c1cccc2.Cl</t>
+  </si>
+  <si>
+    <t>[4.05]</t>
+  </si>
+  <si>
+    <t>3.138999938964844</t>
+  </si>
+  <si>
+    <t>287.744</t>
+  </si>
+  <si>
+    <t>119.7</t>
+  </si>
+  <si>
+    <t>16</t>
+  </si>
+  <si>
+    <t>COc1cccc(c1)Nc2c3ccccc3ncn2.Cl</t>
+  </si>
+  <si>
+    <t>1865544</t>
+  </si>
+  <si>
+    <t>OCCNc1ncnc2c1c(c1ccccc1)c(o2)c1ccccc1</t>
+  </si>
+  <si>
+    <t>[4.294]</t>
+  </si>
+  <si>
+    <t>3.0820000171661377</t>
+  </si>
+  <si>
+    <t>331.36800000000005</t>
+  </si>
+  <si>
+    <t>159.0</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>71</t>
+  </si>
+  <si>
+    <t>c1ccc(cc1)c2c3c(ncnc3oc2c4ccccc4)NCCO</t>
+  </si>
+  <si>
+    <t>1415762</t>
+  </si>
+  <si>
+    <t>c1ccc(cc1)CSc1nnc(o1)c1ccncc1</t>
+  </si>
+  <si>
+    <t>[4.902]</t>
+  </si>
+  <si>
+    <t>3.3059999942779537</t>
+  </si>
+  <si>
+    <t>269.322</t>
+  </si>
+  <si>
+    <t>170.0</t>
+  </si>
+  <si>
+    <t>30</t>
+  </si>
+  <si>
+    <t>17</t>
+  </si>
+  <si>
+    <t>c1ccc(cc1)CSc2nnc(o2)c3ccncc3</t>
+  </si>
+  <si>
+    <t>1444229</t>
+  </si>
+  <si>
+    <t>FC(c1cccc(c1)Nc1ncnc2c1cccc2)(F)F</t>
+  </si>
+  <si>
+    <t>3.2689995765686035</t>
+  </si>
+  <si>
+    <t>289.255</t>
+  </si>
+  <si>
+    <t>101.0</t>
+  </si>
+  <si>
+    <t>355.0</t>
+  </si>
+  <si>
+    <t>c1ccc2c(c1)c(ncn2)Nc3cccc(c3)C(F)(F)F</t>
+  </si>
+  <si>
+    <t>1327907</t>
+  </si>
+  <si>
+    <t>O=C(c1cccs1)Nc1nnc(s1)Cc1ccccc1</t>
+  </si>
+  <si>
+    <t>[7.12]</t>
+  </si>
+  <si>
+    <t>3.6050002574920654</t>
+  </si>
+  <si>
+    <t>301.387</t>
+  </si>
+  <si>
+    <t>379.0</t>
+  </si>
+  <si>
+    <t>18</t>
+  </si>
+  <si>
+    <t>c1ccc(cc1)Cc2nnc(s2)NC(=O)c3cccs3</t>
+  </si>
+  <si>
+    <t>1228629</t>
+  </si>
+  <si>
+    <t>Clc1ccc(cc1)CNc1ncnc2c1cccc2</t>
+  </si>
+  <si>
+    <t>[5.564]</t>
+  </si>
+  <si>
+    <t>3.523000240325928</t>
+  </si>
+  <si>
+    <t>269.72900000000004</t>
+  </si>
+  <si>
+    <t>415.5</t>
+  </si>
+  <si>
+    <t>c1ccc2c(c1)c(ncn2)NCc3ccc(cc3)Cl</t>
+  </si>
+  <si>
+    <t>30719859</t>
+  </si>
+  <si>
+    <t>Clc1ccc(o1)C(=O)Nc1ccccc1N1CCCCC1</t>
+  </si>
+  <si>
+    <t>[5.346]</t>
+  </si>
+  <si>
+    <t>3.794999837875366</t>
+  </si>
+  <si>
+    <t>304.771</t>
+  </si>
+  <si>
+    <t>424.3</t>
+  </si>
+  <si>
+    <t>19</t>
+  </si>
+  <si>
+    <t>c1ccc(c(c1)NC(=O)c2ccc(o2)Cl)N3CCCCC3</t>
+  </si>
+  <si>
+    <t>18908671</t>
+  </si>
+  <si>
+    <t>Cc1ccc(cc1)S(=O)(=O)Nc1cccc(c1)C(F)(F)F</t>
+  </si>
+  <si>
+    <t>[7.903]</t>
+  </si>
+  <si>
+    <t>3.747999668121338</t>
+  </si>
+  <si>
+    <t>315.311</t>
+  </si>
+  <si>
+    <t>527.0</t>
+  </si>
+  <si>
+    <t>24</t>
+  </si>
+  <si>
+    <t>Cc1ccc(cc1)S(=O)(=O)Nc2cccc(c2)C(F)(F)F</t>
+  </si>
+  <si>
+    <t>1377874</t>
+  </si>
+  <si>
+    <t>O=C1S/C(=C/c2ccc(o2)c2ccc(c(c2)Cl)F)/C(=O)N1</t>
+  </si>
+  <si>
+    <t>[8.052]</t>
+  </si>
+  <si>
+    <t>3.9079997539520255</t>
+  </si>
+  <si>
+    <t>323.7270000000001</t>
+  </si>
+  <si>
+    <t>125.0</t>
   </si>
   <si>
     <t>20</t>
   </si>
   <si>
-    <t>c1cc(c(c(c1)Cl)NC(=O)c2ccncc2)Cl</t>
-  </si>
-  <si>
-    <t>3605943</t>
-  </si>
-  <si>
-    <t>COc1cccc(c1)Nc1ncnc2c1cccc2.Cl</t>
-  </si>
-  <si>
-    <t>[4.05]</t>
-  </si>
-  <si>
-    <t>3.138999938964844</t>
-  </si>
-  <si>
-    <t>287.744</t>
-  </si>
-  <si>
-    <t>119.7</t>
-  </si>
-  <si>
-    <t>16</t>
-  </si>
-  <si>
-    <t>COc1cccc(c1)Nc2c3ccccc3ncn2.Cl</t>
-  </si>
-  <si>
-    <t>1865544</t>
-  </si>
-  <si>
-    <t>OCCNc1ncnc2c1c(c1ccccc1)c(o2)c1ccccc1</t>
-  </si>
-  <si>
-    <t>[4.294]</t>
-  </si>
-  <si>
-    <t>3.0820000171661377</t>
-  </si>
-  <si>
-    <t>331.36800000000005</t>
-  </si>
-  <si>
-    <t>159.0</t>
-  </si>
-  <si>
-    <t>5</t>
-  </si>
-  <si>
-    <t>71</t>
-  </si>
-  <si>
-    <t>c1ccc(cc1)c2c3c(ncnc3oc2c4ccccc4)NCCO</t>
-  </si>
-  <si>
-    <t>1415762</t>
-  </si>
-  <si>
-    <t>c1ccc(cc1)CSc1nnc(o1)c1ccncc1</t>
-  </si>
-  <si>
-    <t>[4.902]</t>
-  </si>
-  <si>
-    <t>3.3059999942779537</t>
-  </si>
-  <si>
-    <t>269.322</t>
-  </si>
-  <si>
-    <t>170.0</t>
-  </si>
-  <si>
-    <t>30</t>
-  </si>
-  <si>
-    <t>17</t>
-  </si>
-  <si>
-    <t>c1ccc(cc1)CSc2nnc(o2)c3ccncc3</t>
-  </si>
-  <si>
-    <t>1444229</t>
-  </si>
-  <si>
-    <t>O=C(Nc1noc(c1)C(C)(C)C)Nc1ccc(cc1)F</t>
-  </si>
-  <si>
-    <t>[3.417]</t>
-  </si>
-  <si>
-    <t>3.4079995155334477</t>
-  </si>
-  <si>
-    <t>277.29400000000004</t>
-  </si>
-  <si>
-    <t>114.0</t>
-  </si>
-  <si>
-    <t>CC(C)(C)c1cc(no1)NC(=O)Nc2ccc(cc2)F</t>
-  </si>
-  <si>
-    <t>2546448</t>
-  </si>
-  <si>
-    <t>O=C(c1cccs1)Nc1nnc(s1)Cc1ccccc1</t>
-  </si>
-  <si>
-    <t>[7.12]</t>
-  </si>
-  <si>
-    <t>3.6050002574920654</t>
-  </si>
-  <si>
-    <t>301.387</t>
-  </si>
-  <si>
-    <t>379.0</t>
-  </si>
-  <si>
-    <t>18</t>
-  </si>
-  <si>
-    <t>c1ccc(cc1)Cc2nnc(s2)NC(=O)c3cccs3</t>
-  </si>
-  <si>
-    <t>1228629</t>
-  </si>
-  <si>
-    <t>Clc1ccc(cc1)CNc1ncnc2c1cccc2</t>
-  </si>
-  <si>
-    <t>[5.564]</t>
-  </si>
-  <si>
-    <t>3.523000240325928</t>
-  </si>
-  <si>
-    <t>269.72900000000004</t>
-  </si>
-  <si>
-    <t>415.5</t>
-  </si>
-  <si>
-    <t>c1ccc2c(c1)c(ncn2)NCc3ccc(cc3)Cl</t>
-  </si>
-  <si>
-    <t>30719859</t>
-  </si>
-  <si>
-    <t>Clc1ccc(o1)C(=O)Nc1ccccc1N1CCCCC1</t>
-  </si>
-  <si>
-    <t>[5.346]</t>
-  </si>
-  <si>
-    <t>3.794999837875366</t>
-  </si>
-  <si>
-    <t>304.771</t>
-  </si>
-  <si>
-    <t>424.3</t>
-  </si>
-  <si>
-    <t>19</t>
-  </si>
-  <si>
-    <t>c1ccc(c(c1)NC(=O)c2ccc(o2)Cl)N3CCCCC3</t>
-  </si>
-  <si>
-    <t>18908671</t>
-  </si>
-  <si>
-    <t>Cc1ccc(cc1)S(=O)(=O)Nc1cccc(c1)C(F)(F)F</t>
-  </si>
-  <si>
-    <t>[7.903]</t>
-  </si>
-  <si>
-    <t>3.747999668121338</t>
-  </si>
-  <si>
-    <t>315.311</t>
-  </si>
-  <si>
-    <t>527.0</t>
-  </si>
-  <si>
-    <t>24</t>
-  </si>
-  <si>
-    <t>Cc1ccc(cc1)S(=O)(=O)Nc2cccc(c2)C(F)(F)F</t>
-  </si>
-  <si>
-    <t>1377874</t>
-  </si>
-  <si>
-    <t>O=C1S/C(=C/c2ccc(o2)c2ccc(c(c2)Cl)F)/C(=O)N1</t>
-  </si>
-  <si>
-    <t>[8.052]</t>
-  </si>
-  <si>
-    <t>3.9079997539520255</t>
-  </si>
-  <si>
-    <t>323.7270000000001</t>
-  </si>
-  <si>
-    <t>125.0</t>
-  </si>
-  <si>
     <t>c1cc(c(cc1c2ccc(o2)/C=C/3\C(=O)NC(=O)S3)Cl)F</t>
   </si>
   <si>
     <t>25775231</t>
   </si>
   <si>
-    <t>Brc1ccc(o1)C(=O)Nc1ccccc1N1CCCCC1</t>
-  </si>
-  <si>
-    <t>3.9770002365112314</t>
-  </si>
-  <si>
-    <t>349.222</t>
-  </si>
-  <si>
-    <t>530.0</t>
-  </si>
-  <si>
-    <t>c1ccc(c(c1)NC(=O)c2ccc(o2)Br)N3CCCCC3</t>
-  </si>
-  <si>
-    <t>1716329</t>
+    <t>Clc1cccc(c1)Nc1ncnc2c1cccc2.Cl</t>
+  </si>
+  <si>
+    <t>3.89900016784668</t>
+  </si>
+  <si>
+    <t>292.163</t>
+  </si>
+  <si>
+    <t>7366.0</t>
+  </si>
+  <si>
+    <t>c1ccc2c(c1)c(ncn2)Nc3cccc(c3)Cl.Cl</t>
+  </si>
+  <si>
+    <t>1859493</t>
+  </si>
+  <si>
+    <t>COc1cc(ccc1OC)c1csc(c1C(=O)OC(C)C)N</t>
+  </si>
+  <si>
+    <t>[10.184]</t>
+  </si>
+  <si>
+    <t>4.079999923706056</t>
+  </si>
+  <si>
+    <t>321.391</t>
+  </si>
+  <si>
+    <t>10117.0</t>
+  </si>
+  <si>
+    <t>21</t>
+  </si>
+  <si>
+    <t>CC(C)OC(=O)c1c(csc1N)c2ccc(c(c2)OC)OC</t>
+  </si>
+  <si>
+    <t>837243</t>
   </si>
   <si>
     <t>FC(c1ccc(cc1)c1nnc2n1nc(cc2)NC1CC1)(F)F</t>
@@ -668,9 +674,6 @@
   </si>
   <si>
     <t>32</t>
-  </si>
-  <si>
-    <t>21</t>
   </si>
   <si>
     <t>c1cc(ccc1c2nnc3n2nc(cc3)NC4CC4)C(F)(F)F</t>
@@ -2331,474 +2334,474 @@
         <v>66</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>67</v>
+        <v>47</v>
       </c>
       <c r="H7" s="2" t="s">
         <v>23</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>58</v>
+        <v>28</v>
       </c>
       <c r="J7" s="2" t="s">
-        <v>68</v>
+        <v>48</v>
       </c>
       <c r="K7" s="2" t="s">
         <v>26</v>
       </c>
       <c r="L7" s="2" t="s">
-        <v>49</v>
+        <v>67</v>
       </c>
       <c r="M7" s="2" t="s">
-        <v>69</v>
+        <v>28</v>
       </c>
       <c r="N7" s="2" t="s">
         <v>29</v>
       </c>
       <c r="O7" s="2" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="P7" s="2" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="8" spans="1:16" s="3" customFormat="1" ht="187.5" customHeight="1">
       <c r="B8" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="D8" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="E8" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="D8" s="3" t="s">
+      <c r="F8" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="E8" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="F8" s="3" t="s">
-        <v>76</v>
-      </c>
       <c r="G8" s="3" t="s">
-        <v>47</v>
+        <v>57</v>
       </c>
       <c r="H8" s="3" t="s">
         <v>23</v>
       </c>
       <c r="I8" s="3" t="s">
-        <v>28</v>
+        <v>75</v>
       </c>
       <c r="J8" s="3" t="s">
-        <v>48</v>
+        <v>76</v>
       </c>
       <c r="K8" s="3" t="s">
         <v>26</v>
       </c>
       <c r="L8" s="3" t="s">
-        <v>77</v>
+        <v>67</v>
       </c>
       <c r="M8" s="3" t="s">
-        <v>28</v>
+        <v>58</v>
       </c>
       <c r="N8" s="3" t="s">
         <v>29</v>
       </c>
       <c r="O8" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="P8" s="3" t="s">
         <v>78</v>
-      </c>
-      <c r="P8" s="3" t="s">
-        <v>79</v>
       </c>
     </row>
     <row r="9" spans="1:16" s="2" customFormat="1" ht="187.5" customHeight="1">
       <c r="B9" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="C9" s="2" t="s">
         <v>80</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>63</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>81</v>
       </c>
       <c r="E9" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="F9" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="F9" s="2" t="s">
+      <c r="G9" s="2" t="s">
         <v>83</v>
-      </c>
-      <c r="G9" s="2" t="s">
-        <v>57</v>
       </c>
       <c r="H9" s="2" t="s">
         <v>23</v>
       </c>
       <c r="I9" s="2" t="s">
-        <v>69</v>
+        <v>75</v>
       </c>
       <c r="J9" s="2" t="s">
-        <v>68</v>
+        <v>84</v>
       </c>
       <c r="K9" s="2" t="s">
         <v>26</v>
       </c>
       <c r="L9" s="2" t="s">
-        <v>77</v>
+        <v>85</v>
       </c>
       <c r="M9" s="2" t="s">
-        <v>58</v>
+        <v>28</v>
       </c>
       <c r="N9" s="2" t="s">
         <v>29</v>
       </c>
       <c r="O9" s="2" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="P9" s="2" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
     </row>
     <row r="10" spans="1:16" s="3" customFormat="1" ht="187.5" customHeight="1">
       <c r="B10" s="3" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>55</v>
+        <v>91</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>67</v>
+        <v>37</v>
       </c>
       <c r="H10" s="3" t="s">
         <v>23</v>
       </c>
       <c r="I10" s="3" t="s">
-        <v>69</v>
+        <v>27</v>
       </c>
       <c r="J10" s="3" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="K10" s="3" t="s">
         <v>26</v>
       </c>
       <c r="L10" s="3" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="M10" s="3" t="s">
-        <v>28</v>
+        <v>58</v>
       </c>
       <c r="N10" s="3" t="s">
         <v>29</v>
       </c>
       <c r="O10" s="3" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="P10" s="3" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
     </row>
     <row r="11" spans="1:16" s="2" customFormat="1" ht="187.5" customHeight="1">
       <c r="B11" s="2" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>37</v>
+        <v>47</v>
       </c>
       <c r="H11" s="2" t="s">
         <v>23</v>
       </c>
       <c r="I11" s="2" t="s">
-        <v>27</v>
+        <v>100</v>
       </c>
       <c r="J11" s="2" t="s">
-        <v>90</v>
+        <v>76</v>
       </c>
       <c r="K11" s="2" t="s">
         <v>26</v>
       </c>
       <c r="L11" s="2" t="s">
-        <v>91</v>
+        <v>101</v>
       </c>
       <c r="M11" s="2" t="s">
-        <v>58</v>
+        <v>28</v>
       </c>
       <c r="N11" s="2" t="s">
         <v>29</v>
       </c>
       <c r="O11" s="2" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="P11" s="2" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
     </row>
     <row r="12" spans="1:16" s="3" customFormat="1" ht="187.5" customHeight="1">
       <c r="B12" s="3" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>47</v>
+        <v>83</v>
       </c>
       <c r="H12" s="3" t="s">
         <v>23</v>
       </c>
       <c r="I12" s="3" t="s">
-        <v>106</v>
+        <v>75</v>
       </c>
       <c r="J12" s="3" t="s">
-        <v>68</v>
+        <v>109</v>
       </c>
       <c r="K12" s="3" t="s">
         <v>26</v>
       </c>
       <c r="L12" s="3" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="M12" s="3" t="s">
-        <v>28</v>
+        <v>58</v>
       </c>
       <c r="N12" s="3" t="s">
         <v>29</v>
       </c>
       <c r="O12" s="3" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="P12" s="3" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
     </row>
     <row r="13" spans="1:16" s="2" customFormat="1" ht="187.5" customHeight="1">
       <c r="B13" s="2" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>67</v>
+        <v>47</v>
       </c>
       <c r="H13" s="2" t="s">
         <v>23</v>
       </c>
       <c r="I13" s="2" t="s">
-        <v>69</v>
+        <v>75</v>
       </c>
       <c r="J13" s="2" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="K13" s="2" t="s">
         <v>26</v>
       </c>
       <c r="L13" s="2" t="s">
-        <v>107</v>
+        <v>118</v>
       </c>
       <c r="M13" s="2" t="s">
-        <v>58</v>
+        <v>28</v>
       </c>
       <c r="N13" s="2" t="s">
         <v>29</v>
       </c>
       <c r="O13" s="2" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="P13" s="2" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
     </row>
     <row r="14" spans="1:16" s="3" customFormat="1" ht="187.5" customHeight="1">
       <c r="B14" s="3" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
       <c r="G14" s="3" t="s">
-        <v>47</v>
+        <v>57</v>
       </c>
       <c r="H14" s="3" t="s">
         <v>23</v>
       </c>
       <c r="I14" s="3" t="s">
-        <v>69</v>
+        <v>28</v>
       </c>
       <c r="J14" s="3" t="s">
-        <v>123</v>
+        <v>59</v>
       </c>
       <c r="K14" s="3" t="s">
         <v>26</v>
       </c>
       <c r="L14" s="3" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="M14" s="3" t="s">
-        <v>28</v>
+        <v>58</v>
       </c>
       <c r="N14" s="3" t="s">
         <v>29</v>
       </c>
       <c r="O14" s="3" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="P14" s="3" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
     </row>
     <row r="15" spans="1:16" s="2" customFormat="1" ht="187.5" customHeight="1">
       <c r="B15" s="2" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>57</v>
+        <v>47</v>
       </c>
       <c r="H15" s="2" t="s">
         <v>23</v>
       </c>
       <c r="I15" s="2" t="s">
-        <v>69</v>
+        <v>75</v>
       </c>
       <c r="J15" s="2" t="s">
-        <v>132</v>
+        <v>84</v>
       </c>
       <c r="K15" s="2" t="s">
         <v>26</v>
       </c>
       <c r="L15" s="2" t="s">
-        <v>124</v>
+        <v>133</v>
       </c>
       <c r="M15" s="2" t="s">
-        <v>58</v>
+        <v>28</v>
       </c>
       <c r="N15" s="2" t="s">
         <v>29</v>
       </c>
       <c r="O15" s="2" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="P15" s="2" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
     </row>
     <row r="16" spans="1:16" s="3" customFormat="1" ht="187.5" customHeight="1">
       <c r="B16" s="3" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="G16" s="3" t="s">
-        <v>47</v>
+        <v>57</v>
       </c>
       <c r="H16" s="3" t="s">
         <v>23</v>
       </c>
       <c r="I16" s="3" t="s">
-        <v>69</v>
+        <v>141</v>
       </c>
       <c r="J16" s="3" t="s">
-        <v>90</v>
+        <v>142</v>
       </c>
       <c r="K16" s="3" t="s">
         <v>26</v>
       </c>
       <c r="L16" s="3" t="s">
-        <v>140</v>
+        <v>133</v>
       </c>
       <c r="M16" s="3" t="s">
-        <v>28</v>
+        <v>58</v>
       </c>
       <c r="N16" s="3" t="s">
         <v>29</v>
       </c>
       <c r="O16" s="3" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="P16" s="3" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
     </row>
     <row r="17" spans="2:16" s="2" customFormat="1" ht="187.5" customHeight="1">
       <c r="B17" s="2" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="G17" s="2" t="s">
         <v>57</v>
@@ -2807,66 +2810,66 @@
         <v>23</v>
       </c>
       <c r="I17" s="2" t="s">
-        <v>148</v>
+        <v>27</v>
       </c>
       <c r="J17" s="2" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="K17" s="2" t="s">
         <v>26</v>
       </c>
       <c r="L17" s="2" t="s">
-        <v>140</v>
+        <v>151</v>
       </c>
       <c r="M17" s="2" t="s">
-        <v>58</v>
+        <v>28</v>
       </c>
       <c r="N17" s="2" t="s">
         <v>29</v>
       </c>
       <c r="O17" s="2" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="P17" s="2" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
     </row>
     <row r="18" spans="2:16" s="3" customFormat="1" ht="187.5" customHeight="1">
       <c r="B18" s="3" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>153</v>
+        <v>129</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="G18" s="3" t="s">
-        <v>57</v>
+        <v>158</v>
       </c>
       <c r="H18" s="3" t="s">
         <v>23</v>
       </c>
       <c r="I18" s="3" t="s">
-        <v>27</v>
+        <v>75</v>
       </c>
       <c r="J18" s="3" t="s">
-        <v>157</v>
+        <v>84</v>
       </c>
       <c r="K18" s="3" t="s">
         <v>26</v>
       </c>
       <c r="L18" s="3" t="s">
-        <v>158</v>
+        <v>151</v>
       </c>
       <c r="M18" s="3" t="s">
-        <v>28</v>
+        <v>58</v>
       </c>
       <c r="N18" s="3" t="s">
         <v>29</v>
@@ -2895,51 +2898,51 @@
         <v>165</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>57</v>
+        <v>47</v>
       </c>
       <c r="H19" s="2" t="s">
         <v>23</v>
       </c>
       <c r="I19" s="2" t="s">
-        <v>148</v>
+        <v>141</v>
       </c>
       <c r="J19" s="2" t="s">
-        <v>140</v>
+        <v>101</v>
       </c>
       <c r="K19" s="2" t="s">
         <v>26</v>
       </c>
       <c r="L19" s="2" t="s">
-        <v>158</v>
+        <v>166</v>
       </c>
       <c r="M19" s="2" t="s">
-        <v>58</v>
+        <v>28</v>
       </c>
       <c r="N19" s="2" t="s">
         <v>29</v>
       </c>
       <c r="O19" s="2" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="P19" s="2" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
     </row>
     <row r="20" spans="2:16" s="3" customFormat="1" ht="187.5" customHeight="1">
       <c r="B20" s="3" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="F20" s="3" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="G20" s="3" t="s">
         <v>47</v>
@@ -2948,19 +2951,19 @@
         <v>23</v>
       </c>
       <c r="I20" s="3" t="s">
-        <v>148</v>
+        <v>75</v>
       </c>
       <c r="J20" s="3" t="s">
-        <v>107</v>
+        <v>84</v>
       </c>
       <c r="K20" s="3" t="s">
         <v>26</v>
       </c>
       <c r="L20" s="3" t="s">
-        <v>173</v>
+        <v>166</v>
       </c>
       <c r="M20" s="3" t="s">
-        <v>28</v>
+        <v>58</v>
       </c>
       <c r="N20" s="3" t="s">
         <v>29</v>
@@ -2995,48 +2998,48 @@
         <v>23</v>
       </c>
       <c r="I21" s="2" t="s">
-        <v>69</v>
+        <v>27</v>
       </c>
       <c r="J21" s="2" t="s">
-        <v>90</v>
+        <v>166</v>
       </c>
       <c r="K21" s="2" t="s">
         <v>26</v>
       </c>
       <c r="L21" s="2" t="s">
-        <v>173</v>
+        <v>181</v>
       </c>
       <c r="M21" s="2" t="s">
-        <v>58</v>
+        <v>28</v>
       </c>
       <c r="N21" s="2" t="s">
         <v>29</v>
       </c>
       <c r="O21" s="2" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="P21" s="2" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
     </row>
     <row r="22" spans="2:16" s="3" customFormat="1" ht="187.5" customHeight="1">
       <c r="B22" s="3" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="F22" s="3" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="G22" s="3" t="s">
-        <v>47</v>
+        <v>57</v>
       </c>
       <c r="H22" s="3" t="s">
         <v>23</v>
@@ -3045,42 +3048,42 @@
         <v>27</v>
       </c>
       <c r="J22" s="3" t="s">
-        <v>173</v>
+        <v>189</v>
       </c>
       <c r="K22" s="3" t="s">
         <v>26</v>
       </c>
       <c r="L22" s="3" t="s">
-        <v>188</v>
+        <v>181</v>
       </c>
       <c r="M22" s="3" t="s">
-        <v>28</v>
+        <v>58</v>
       </c>
       <c r="N22" s="3" t="s">
         <v>29</v>
       </c>
       <c r="O22" s="3" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="P22" s="3" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
     </row>
     <row r="23" spans="2:16" s="2" customFormat="1" ht="187.5" customHeight="1">
       <c r="B23" s="2" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="G23" s="2" t="s">
         <v>57</v>
@@ -3089,36 +3092,36 @@
         <v>23</v>
       </c>
       <c r="I23" s="2" t="s">
-        <v>27</v>
+        <v>58</v>
       </c>
       <c r="J23" s="2" t="s">
-        <v>196</v>
+        <v>38</v>
       </c>
       <c r="K23" s="2" t="s">
         <v>26</v>
       </c>
       <c r="L23" s="2" t="s">
-        <v>188</v>
+        <v>197</v>
       </c>
       <c r="M23" s="2" t="s">
-        <v>58</v>
+        <v>28</v>
       </c>
       <c r="N23" s="2" t="s">
         <v>29</v>
       </c>
       <c r="O23" s="2" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="P23" s="2" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
     </row>
     <row r="24" spans="2:16" s="3" customFormat="1" ht="187.5" customHeight="1">
       <c r="B24" s="3" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>200</v>
+        <v>129</v>
       </c>
       <c r="D24" s="3" t="s">
         <v>201</v>
@@ -3130,7 +3133,7 @@
         <v>203</v>
       </c>
       <c r="G24" s="3" t="s">
-        <v>57</v>
+        <v>37</v>
       </c>
       <c r="H24" s="3" t="s">
         <v>23</v>
@@ -3139,16 +3142,16 @@
         <v>58</v>
       </c>
       <c r="J24" s="3" t="s">
-        <v>38</v>
+        <v>84</v>
       </c>
       <c r="K24" s="3" t="s">
         <v>26</v>
       </c>
       <c r="L24" s="3" t="s">
-        <v>132</v>
+        <v>197</v>
       </c>
       <c r="M24" s="3" t="s">
-        <v>28</v>
+        <v>58</v>
       </c>
       <c r="N24" s="3" t="s">
         <v>29</v>
@@ -3165,16 +3168,16 @@
         <v>206</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>184</v>
+        <v>207</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="G25" s="2" t="s">
         <v>57</v>
@@ -3183,45 +3186,45 @@
         <v>23</v>
       </c>
       <c r="I25" s="2" t="s">
-        <v>27</v>
+        <v>100</v>
       </c>
       <c r="J25" s="2" t="s">
-        <v>173</v>
+        <v>76</v>
       </c>
       <c r="K25" s="2" t="s">
         <v>26</v>
       </c>
       <c r="L25" s="2" t="s">
-        <v>132</v>
+        <v>211</v>
       </c>
       <c r="M25" s="2" t="s">
-        <v>58</v>
+        <v>28</v>
       </c>
       <c r="N25" s="2" t="s">
         <v>29</v>
       </c>
       <c r="O25" s="2" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="P25" s="2" t="s">
-        <v>211</v>
+        <v>213</v>
       </c>
     </row>
     <row r="26" spans="2:16" s="3" customFormat="1" ht="187.5" customHeight="1">
       <c r="B26" s="3" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>213</v>
+        <v>215</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>214</v>
+        <v>216</v>
       </c>
       <c r="E26" s="3" t="s">
-        <v>215</v>
+        <v>217</v>
       </c>
       <c r="F26" s="3" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
       <c r="G26" s="3" t="s">
         <v>37</v>
@@ -3233,45 +3236,45 @@
         <v>27</v>
       </c>
       <c r="J26" s="3" t="s">
-        <v>217</v>
+        <v>219</v>
       </c>
       <c r="K26" s="3" t="s">
         <v>26</v>
       </c>
       <c r="L26" s="3" t="s">
-        <v>218</v>
+        <v>211</v>
       </c>
       <c r="M26" s="3" t="s">
-        <v>28</v>
+        <v>58</v>
       </c>
       <c r="N26" s="3" t="s">
         <v>29</v>
       </c>
       <c r="O26" s="3" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="P26" s="3" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
     </row>
     <row r="27" spans="2:16" s="2" customFormat="1" ht="187.5" customHeight="1">
       <c r="B27" s="2" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="F27" s="2" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="G27" s="2" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="H27" s="2" t="s">
         <v>23</v>
@@ -3280,13 +3283,13 @@
         <v>58</v>
       </c>
       <c r="J27" s="2" t="s">
-        <v>196</v>
+        <v>189</v>
       </c>
       <c r="K27" s="2" t="s">
         <v>26</v>
       </c>
       <c r="L27" s="2" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="M27" s="2" t="s">
         <v>28</v>
@@ -3295,10 +3298,10 @@
         <v>29</v>
       </c>
       <c r="O27" s="2" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="P27" s="2" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
     </row>
   </sheetData>

</xml_diff>